<commit_message>
worked on nipa add factors
</commit_message>
<xml_diff>
--- a/development/features/nipa-consistent-FIM/results/11-2020/data/fim_interactive.xlsx
+++ b/development/features/nipa-consistent-FIM/results/11-2020/data/fim_interactive.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,19 +422,19 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.0301973156737349</v>
+        <v>0.4860680840188342</v>
       </c>
       <c r="F2">
-        <v>-0.4350874079146171</v>
+        <v>0.08169024292858429</v>
       </c>
       <c r="G2">
-        <v>0.1743286394277914</v>
+        <v>0.4946888839019331</v>
       </c>
       <c r="H2">
-        <v>0.1959327382019484</v>
+        <v>0.6371181255487443</v>
       </c>
       <c r="I2">
-        <v>-0.4004586933034747</v>
+        <v>-0.6457389254318432</v>
       </c>
     </row>
     <row r="3">
@@ -455,19 +455,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-1.886918388454525</v>
+        <v>-1.371672358118625</v>
       </c>
       <c r="F3">
-        <v>-0.7355357359278551</v>
+        <v>-0.2210374419742249</v>
       </c>
       <c r="G3">
-        <v>-1.417109040797517</v>
+        <v>-0.6648250072254314</v>
       </c>
       <c r="H3">
-        <v>0.1443572750032584</v>
+        <v>0.1590883676069691</v>
       </c>
       <c r="I3">
-        <v>-0.6141666226602664</v>
+        <v>-0.8659357185001628</v>
       </c>
     </row>
     <row r="4">
@@ -488,19 +488,19 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>-0.3094652848658663</v>
+        <v>0.1759225440194582</v>
       </c>
       <c r="F4">
-        <v>-0.6022373754700017</v>
+        <v>-0.09483571422655872</v>
       </c>
       <c r="G4">
-        <v>0.4282649627284007</v>
+        <v>0.7419382413465793</v>
       </c>
       <c r="H4">
-        <v>-0.4682870513075125</v>
+        <v>-0.03911689401130113</v>
       </c>
       <c r="I4">
-        <v>-0.2694431962867544</v>
+        <v>-0.52689880331582</v>
       </c>
     </row>
     <row r="5">
@@ -521,19 +521,19 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>-1.099670111084927</v>
+        <v>-0.6478944774693745</v>
       </c>
       <c r="F5">
-        <v>-0.8315627750197636</v>
+        <v>-0.3393940518874268</v>
       </c>
       <c r="G5">
-        <v>-0.4919310908151831</v>
+        <v>-0.8358291621042218</v>
       </c>
       <c r="H5">
-        <v>-0.5229946480911283</v>
+        <v>0.5299153898310077</v>
       </c>
       <c r="I5">
-        <v>-0.08474437217861565</v>
+        <v>-0.3419807051961604</v>
       </c>
     </row>
     <row r="6">
@@ -554,19 +554,19 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>-0.2162355418791546</v>
+        <v>0.1997162826664242</v>
       </c>
       <c r="F6">
-        <v>-0.8780723315711185</v>
+        <v>-0.4109820022255293</v>
       </c>
       <c r="G6">
-        <v>-0.2174007110986757</v>
+        <v>-0.004798706463803183</v>
       </c>
       <c r="H6">
-        <v>-0.02371134001018647</v>
+        <v>0.4375539874872086</v>
       </c>
       <c r="I6">
-        <v>0.02487650922970756</v>
+        <v>-0.2330389983569812</v>
       </c>
     </row>
     <row r="7">
@@ -587,19 +587,19 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.6965505858098224</v>
+        <v>1.083400276500031</v>
       </c>
       <c r="F7">
-        <v>-0.2322050880050318</v>
+        <v>0.2027861564291348</v>
       </c>
       <c r="G7">
-        <v>0.6071382455658475</v>
+        <v>0.1167020212982178</v>
       </c>
       <c r="H7">
-        <v>-0.1548344774092804</v>
+        <v>0.9814371046878589</v>
       </c>
       <c r="I7">
-        <v>0.2442468176532554</v>
+        <v>-0.01473884948604593</v>
       </c>
     </row>
     <row r="8">
@@ -620,19 +620,19 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1.045407526675324</v>
+        <v>1.410483524419149</v>
       </c>
       <c r="F8">
-        <v>0.1065131148802657</v>
+        <v>0.5114264015290575</v>
       </c>
       <c r="G8">
-        <v>0.4269529048802224</v>
+        <v>-0.005555307703252244</v>
       </c>
       <c r="H8">
-        <v>0.2218869860807692</v>
+        <v>1.277767859852481</v>
       </c>
       <c r="I8">
-        <v>0.3965676357143323</v>
+        <v>0.1382709722699202</v>
       </c>
     </row>
     <row r="9">
@@ -653,19 +653,19 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.8419643655441872</v>
+        <v>1.183725376435222</v>
       </c>
       <c r="F9">
-        <v>0.5919217340375442</v>
+        <v>0.9693313650052067</v>
       </c>
       <c r="G9">
-        <v>-0.3310317054594185</v>
+        <v>0.3314497821167763</v>
       </c>
       <c r="H9">
-        <v>-0.3383335145008904</v>
+        <v>-0.4053306945159103</v>
       </c>
       <c r="I9">
-        <v>1.511329585504496</v>
+        <v>1.257606288834356</v>
       </c>
     </row>
     <row r="10">
@@ -686,19 +686,19 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1.896823328363197</v>
+        <v>2.220962917816165</v>
       </c>
       <c r="F10">
-        <v>1.120186451598132</v>
+        <v>1.474643023792642</v>
       </c>
       <c r="G10">
-        <v>0.4667831920459469</v>
+        <v>-0.1344040332508526</v>
       </c>
       <c r="H10">
-        <v>0.1898815753046091</v>
+        <v>1.355077793805707</v>
       </c>
       <c r="I10">
-        <v>1.240158561012641</v>
+        <v>1.00028915726131</v>
       </c>
     </row>
     <row r="11">
@@ -719,19 +719,19 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2.265792202677162</v>
+        <v>2.58682684924151</v>
       </c>
       <c r="F11">
-        <v>1.512496855814967</v>
+        <v>1.850499666978012</v>
       </c>
       <c r="G11">
-        <v>1.049680143747881</v>
+        <v>0.3783184320669671</v>
       </c>
       <c r="H11">
-        <v>-0.2940141605228076</v>
+        <v>0.9206418771130547</v>
       </c>
       <c r="I11">
-        <v>1.510126219452088</v>
+        <v>1.287866540061488</v>
       </c>
     </row>
     <row r="12">
@@ -752,19 +752,19 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1.893505643625337</v>
+        <v>2.219840859915202</v>
       </c>
       <c r="F12">
-        <v>1.72452138505247</v>
+        <v>2.052839000852025</v>
       </c>
       <c r="G12">
-        <v>0.2570517267989404</v>
+        <v>0.5148298247743641</v>
       </c>
       <c r="H12">
-        <v>-0.1980832680058238</v>
+        <v>0.07245834106173334</v>
       </c>
       <c r="I12">
-        <v>1.83453718483222</v>
+        <v>1.632552694079104</v>
       </c>
     </row>
     <row r="13">
@@ -785,19 +785,19 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1.415055062552841</v>
+        <v>1.751900595527874</v>
       </c>
       <c r="F13">
-        <v>1.867794059304633</v>
+        <v>2.194882805625188</v>
       </c>
       <c r="G13">
-        <v>0.07520069290482989</v>
+        <v>0.1871948514362173</v>
       </c>
       <c r="H13">
-        <v>-0.1843917419515624</v>
+        <v>0.2215417545996476</v>
       </c>
       <c r="I13">
-        <v>1.524246111599573</v>
+        <v>1.34316398949201</v>
       </c>
     </row>
     <row r="14">
@@ -818,19 +818,19 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1.271310149807467</v>
+        <v>1.621088782754319</v>
       </c>
       <c r="F14">
-        <v>1.711415764665701</v>
+        <v>2.044914271859726</v>
       </c>
       <c r="G14">
-        <v>0.3411086127580752</v>
+        <v>0.3438176679836201</v>
       </c>
       <c r="H14">
-        <v>-0.2528969465227389</v>
+        <v>0.2552844291665327</v>
       </c>
       <c r="I14">
-        <v>1.183098483572131</v>
+        <v>1.021986685604166</v>
       </c>
     </row>
     <row r="15">
@@ -851,19 +851,19 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0.7767005046887732</v>
+        <v>1.142802613299667</v>
       </c>
       <c r="F15">
-        <v>1.339142840168604</v>
+        <v>1.683908212874266</v>
       </c>
       <c r="G15">
-        <v>-0.116530367991746</v>
+        <v>0.4682780350108303</v>
       </c>
       <c r="H15">
-        <v>-0.3047403093575179</v>
+        <v>-0.3784882380687687</v>
       </c>
       <c r="I15">
-        <v>1.197971182038037</v>
+        <v>1.053012816357605</v>
       </c>
     </row>
     <row r="16">
@@ -884,19 +884,19 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1.325037655278389</v>
+        <v>1.711627746230585</v>
       </c>
       <c r="F16">
-        <v>1.197025843081867</v>
+        <v>1.556854934453111</v>
       </c>
       <c r="G16">
-        <v>1.75702279865995</v>
+        <v>-0.05414525130185377</v>
       </c>
       <c r="H16">
-        <v>-1.526329075036884</v>
+        <v>0.8001125511799414</v>
       </c>
       <c r="I16">
-        <v>1.094343931655323</v>
+        <v>0.9656604463524974</v>
       </c>
     </row>
     <row r="17">
@@ -917,19 +917,19 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.519779127262337</v>
+        <v>0.9219935635239525</v>
       </c>
       <c r="F17">
-        <v>0.9732068592592411</v>
+        <v>1.349378176452131</v>
       </c>
       <c r="G17">
-        <v>-0.2402570822502153</v>
+        <v>-0.0599874683905746</v>
       </c>
       <c r="H17">
-        <v>-0.09222874926885571</v>
+        <v>0.2420652624995633</v>
       </c>
       <c r="I17">
-        <v>0.8522649587814081</v>
+        <v>0.7399157694149637</v>
       </c>
     </row>
     <row r="18">
@@ -950,19 +950,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0.668068001617887</v>
+        <v>1.081216941298442</v>
       </c>
       <c r="F18">
-        <v>0.8223963222118461</v>
+        <v>1.214410216088162</v>
       </c>
       <c r="G18">
-        <v>0.286609846233455</v>
+        <v>0.5174208495565489</v>
       </c>
       <c r="H18">
-        <v>-0.3243338075920826</v>
+        <v>-0.04216530301556628</v>
       </c>
       <c r="I18">
-        <v>0.7057919629765147</v>
+        <v>0.605961394757459</v>
       </c>
     </row>
     <row r="19">
@@ -983,19 +983,19 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.111108504238281</v>
+        <v>0.5389062440544415</v>
       </c>
       <c r="F19">
-        <v>0.6559983220992232</v>
+        <v>1.063436123776855</v>
       </c>
       <c r="G19">
-        <v>-0.2792950832377376</v>
+        <v>0.6358926447898382</v>
       </c>
       <c r="H19">
-        <v>0.1087444925073918</v>
+        <v>-0.2879900418715545</v>
       </c>
       <c r="I19">
-        <v>0.2816590949686268</v>
+        <v>0.1910036411361578</v>
       </c>
     </row>
     <row r="20">
@@ -1016,19 +1016,19 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>-0.1221173408662013</v>
+        <v>0.3173746368420697</v>
       </c>
       <c r="F20">
-        <v>0.2942095730630755</v>
+        <v>0.7148728464297265</v>
       </c>
       <c r="G20">
-        <v>-0.2368611631781869</v>
+        <v>0.3082253456677642</v>
       </c>
       <c r="H20">
-        <v>-0.08018423422003418</v>
+        <v>-0.09817299882337999</v>
       </c>
       <c r="I20">
-        <v>0.1949280565320197</v>
+        <v>0.1073222899976856</v>
       </c>
     </row>
     <row r="21">
@@ -1049,19 +1049,19 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.537236255478833</v>
+        <v>-0.08573413790691828</v>
       </c>
       <c r="F21">
-        <v>0.02995572737778304</v>
+        <v>0.4629409210720088</v>
       </c>
       <c r="G21">
-        <v>-0.09434222425994124</v>
+        <v>0.4579664561789401</v>
       </c>
       <c r="H21">
-        <v>-0.2972223565920764</v>
+        <v>-0.3143444540806857</v>
       </c>
       <c r="I21">
-        <v>-0.1456716746268154</v>
+        <v>-0.2293561400051727</v>
       </c>
     </row>
     <row r="22">
@@ -1082,19 +1082,19 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>-0.7200914007569256</v>
+        <v>-0.2628872078393714</v>
       </c>
       <c r="F22">
-        <v>-0.3170841232159201</v>
+        <v>0.1269148837875556</v>
       </c>
       <c r="G22">
-        <v>-0.354228921005131</v>
+        <v>-0.04764254032958169</v>
       </c>
       <c r="H22">
-        <v>-0.2315469582366401</v>
+        <v>0.001415114232938797</v>
       </c>
       <c r="I22">
-        <v>-0.1343155215151545</v>
+        <v>-0.2166597817427285</v>
       </c>
     </row>
     <row r="23">
@@ -1115,19 +1115,19 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>-0.6324808434686369</v>
+        <v>-0.1929735086194312</v>
       </c>
       <c r="F23">
-        <v>-0.5029814601426496</v>
+        <v>-0.05605505438091263</v>
       </c>
       <c r="G23">
-        <v>0.1433313278220677</v>
+        <v>0.2259279932006186</v>
       </c>
       <c r="H23">
-        <v>-0.2798215857815144</v>
+        <v>0.1608372538410204</v>
       </c>
       <c r="I23">
-        <v>-0.4959905855091901</v>
+        <v>-0.5797387556610701</v>
       </c>
     </row>
     <row r="24">
@@ -1148,19 +1148,19 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>-1.026250520745382</v>
+        <v>-0.6103157593894319</v>
       </c>
       <c r="F24">
-        <v>-0.7290147551124448</v>
+        <v>-0.2879776534387881</v>
       </c>
       <c r="G24">
-        <v>-0.3133365219176708</v>
+        <v>-0.01692944836407308</v>
       </c>
       <c r="H24">
-        <v>-0.2333033524291203</v>
+        <v>-0.02771452247742881</v>
       </c>
       <c r="I24">
-        <v>-0.4796106463985914</v>
+        <v>-0.5656717885479301</v>
       </c>
     </row>
     <row r="25">
@@ -1181,19 +1181,19 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>-0.7460708966706079</v>
+        <v>-0.3493488708901814</v>
       </c>
       <c r="F25">
-        <v>-0.7812234154103885</v>
+        <v>-0.3538813366846038</v>
       </c>
       <c r="G25">
-        <v>-0.4176496452310299</v>
+        <v>0.6052185045210049</v>
       </c>
       <c r="H25">
-        <v>0.1855587821232748</v>
+        <v>-0.3502867946894414</v>
       </c>
       <c r="I25">
-        <v>-0.5139800335628528</v>
+        <v>-0.6042805807217448</v>
       </c>
     </row>
     <row r="26">
@@ -1214,19 +1214,19 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>-0.8593238854567973</v>
+        <v>-0.487744473636487</v>
       </c>
       <c r="F26">
-        <v>-0.8160315365853565</v>
+        <v>-0.4100956531338827</v>
       </c>
       <c r="G26">
-        <v>-0.3035828970078438</v>
+        <v>0.0710785709364128</v>
       </c>
       <c r="H26">
-        <v>-0.1034767111838284</v>
+        <v>-0.008790751509518233</v>
       </c>
       <c r="I26">
-        <v>-0.4522642772651251</v>
+        <v>-0.5500322930633815</v>
       </c>
     </row>
     <row r="27">
@@ -1247,19 +1247,19 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>-0.08656581830113064</v>
+        <v>0.2622541281363634</v>
       </c>
       <c r="F27">
-        <v>-0.67955278029348</v>
+        <v>-0.296288743944934</v>
       </c>
       <c r="G27">
-        <v>0.4051786280982787</v>
+        <v>0.864000865716967</v>
       </c>
       <c r="H27">
-        <v>0.1142421170401921</v>
+        <v>0.1069422092253407</v>
       </c>
       <c r="I27">
-        <v>-0.6059865634396014</v>
+        <v>-0.7086889468059443</v>
       </c>
     </row>
     <row r="28">
@@ -1280,19 +1280,19 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>-1.122604385854955</v>
+        <v>-0.7925281224231595</v>
       </c>
       <c r="F28">
-        <v>-0.7036412465708731</v>
+        <v>-0.3418418347033659</v>
       </c>
       <c r="G28">
-        <v>-0.5731296339090648</v>
+        <v>-0.06876734097878898</v>
       </c>
       <c r="H28">
-        <v>0.1158303780884188</v>
+        <v>0.04683716166181404</v>
       </c>
       <c r="I28">
-        <v>-0.6653051300343092</v>
+        <v>-0.7705979431061846</v>
       </c>
     </row>
     <row r="29">
@@ -1313,19 +1313,19 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>-0.8149030378977276</v>
+        <v>-0.5121193837178903</v>
       </c>
       <c r="F29">
-        <v>-0.720849281877653</v>
+        <v>-0.3825344629102931</v>
       </c>
       <c r="G29">
-        <v>-0.4403854858461838</v>
+        <v>-0.3078566212245543</v>
       </c>
       <c r="H29">
-        <v>-0.082852069115847</v>
+        <v>0.1955365206213519</v>
       </c>
       <c r="I29">
-        <v>-0.2916654829356968</v>
+        <v>-0.3997992831146879</v>
       </c>
     </row>
     <row r="30">
@@ -1346,19 +1346,19 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>-0.07218541959382402</v>
+        <v>0.2049814903998495</v>
       </c>
       <c r="F30">
-        <v>-0.5240646654119097</v>
+        <v>-0.209352971901209</v>
       </c>
       <c r="G30">
-        <v>-0.2884054451162221</v>
+        <v>0.9226561346382511</v>
       </c>
       <c r="H30">
-        <v>0.5316678259262768</v>
+        <v>-0.2958138659857579</v>
       </c>
       <c r="I30">
-        <v>-0.3154478004038788</v>
+        <v>-0.4218607782526437</v>
       </c>
     </row>
     <row r="31">
@@ -1379,19 +1379,19 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>-0.6006588175423173</v>
+        <v>-0.3379776391562322</v>
       </c>
       <c r="F31">
-        <v>-0.6525879152222064</v>
+        <v>-0.359410913724358</v>
       </c>
       <c r="G31">
-        <v>0.08032406354209809</v>
+        <v>-0.6207245674312992</v>
       </c>
       <c r="H31">
-        <v>-0.3371205342589448</v>
+        <v>0.732959001454615</v>
       </c>
       <c r="I31">
-        <v>-0.3438623468254705</v>
+        <v>-0.450212073179548</v>
       </c>
     </row>
     <row r="32">
@@ -1412,19 +1412,19 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.06717102114142542</v>
+        <v>0.3315455691587478</v>
       </c>
       <c r="F32">
-        <v>-0.3551440634731112</v>
+        <v>-0.07839249082888111</v>
       </c>
       <c r="G32">
-        <v>0.3261788948701952</v>
+        <v>0.418573520434026</v>
       </c>
       <c r="H32">
-        <v>0.001842903029057821</v>
+        <v>0.2797885772831269</v>
       </c>
       <c r="I32">
-        <v>-0.2608507767578276</v>
+        <v>-0.366816528558405</v>
       </c>
     </row>
     <row r="33">
@@ -1445,19 +1445,19 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>-0.06038799814625573</v>
+        <v>0.2065218654663605</v>
       </c>
       <c r="F33">
-        <v>-0.1665153035352432</v>
+        <v>0.1012678214671816</v>
       </c>
       <c r="G33">
-        <v>-0.07398651123223843</v>
+        <v>0.3870676995564565</v>
       </c>
       <c r="H33">
-        <v>0.05390688865936979</v>
+        <v>-0.03570683215632572</v>
       </c>
       <c r="I33">
-        <v>-0.0403083755733871</v>
+        <v>-0.1448390019337704</v>
       </c>
     </row>
     <row r="34">
@@ -1478,19 +1478,19 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0.2808439273863743</v>
+        <v>0.5464523108517716</v>
       </c>
       <c r="F34">
-        <v>-0.0782579667901936</v>
+        <v>0.1866355265801621</v>
       </c>
       <c r="G34">
-        <v>0.08102702624943922</v>
+        <v>0.7074003985694142</v>
       </c>
       <c r="H34">
-        <v>0.1611702090860873</v>
+        <v>-0.09925456184085245</v>
       </c>
       <c r="I34">
-        <v>0.03864669205084783</v>
+        <v>-0.0616935258767901</v>
       </c>
     </row>
     <row r="35">
@@ -1511,19 +1511,19 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>-0.07783243930686226</v>
+        <v>0.1903493090574912</v>
       </c>
       <c r="F35">
-        <v>0.05244862776867015</v>
+        <v>0.318717263633593</v>
       </c>
       <c r="G35">
-        <v>0.314116753371319</v>
+        <v>0.3997191853271509</v>
       </c>
       <c r="H35">
-        <v>-0.4977353637286239</v>
+        <v>-0.2220240185508833</v>
       </c>
       <c r="I35">
-        <v>0.1057861710504426</v>
+        <v>0.01265414228122355</v>
       </c>
     </row>
     <row r="36">
@@ -1544,19 +1544,19 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>2.583795592486665</v>
+        <v>2.845065979591275</v>
       </c>
       <c r="F36">
-        <v>0.6816047706049801</v>
+        <v>0.9470973662417246</v>
       </c>
       <c r="G36">
-        <v>0.5168602701452208</v>
+        <v>0.5995147324770616</v>
       </c>
       <c r="H36">
-        <v>-0.1832625962806899</v>
+        <v>0.08448158673897618</v>
       </c>
       <c r="I36">
-        <v>2.250197918622134</v>
+        <v>2.161069660375237</v>
       </c>
     </row>
     <row r="37">
@@ -1577,19 +1577,19 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1.354967075312305</v>
+        <v>1.608620628598759</v>
       </c>
       <c r="F37">
-        <v>1.03544353896962</v>
+        <v>1.297622057024824</v>
       </c>
       <c r="G37">
-        <v>-0.06473972963780637</v>
+        <v>0.6723462386505684</v>
       </c>
       <c r="H37">
-        <v>0.3713250054579429</v>
+        <v>-0.03445495981190488</v>
       </c>
       <c r="I37">
-        <v>1.048381799492169</v>
+        <v>0.9707293497600957</v>
       </c>
     </row>
     <row r="38">
@@ -1610,19 +1610,19 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>1.546684341069176</v>
+        <v>1.786592397977966</v>
       </c>
       <c r="F38">
-        <v>1.351903642390321</v>
+        <v>1.607657078806373</v>
       </c>
       <c r="G38">
-        <v>0.6893475391488096</v>
+        <v>-0.06298272824822171</v>
       </c>
       <c r="H38">
-        <v>-0.4716557489484011</v>
+        <v>0.592144784436984</v>
       </c>
       <c r="I38">
-        <v>1.328992550868767</v>
+        <v>1.257430341789204</v>
       </c>
     </row>
     <row r="39">
@@ -1643,19 +1643,19 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>3.491945705546649</v>
+        <v>3.708314657848255</v>
       </c>
       <c r="F39">
-        <v>2.244348178603698</v>
+        <v>2.487148416004064</v>
       </c>
       <c r="G39">
-        <v>1.594139837567952</v>
+        <v>-0.9401670276868019</v>
       </c>
       <c r="H39">
-        <v>-0.9772233582420389</v>
+        <v>1.84289552569623</v>
       </c>
       <c r="I39">
-        <v>2.875029226220736</v>
+        <v>2.805586159838827</v>
       </c>
     </row>
     <row r="40">
@@ -1676,19 +1676,19 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>2.840689464984882</v>
+        <v>3.04604572435814</v>
       </c>
       <c r="F40">
-        <v>2.308571646728252</v>
+        <v>2.53739335219578</v>
       </c>
       <c r="G40">
-        <v>2.077543945887875</v>
+        <v>-0.6923124432083195</v>
       </c>
       <c r="H40">
-        <v>-1.140848068104847</v>
+        <v>1.895108765228772</v>
       </c>
       <c r="I40">
-        <v>1.903993587201854</v>
+        <v>1.843249402337687</v>
       </c>
     </row>
     <row r="41">
@@ -1709,19 +1709,19 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2.793670460295999</v>
+        <v>2.988946291211512</v>
       </c>
       <c r="F41">
-        <v>2.668247492974175</v>
+        <v>2.882474767848968</v>
       </c>
       <c r="G41">
-        <v>0.03360594807682363</v>
+        <v>0.4314364861980995</v>
       </c>
       <c r="H41">
-        <v>-0.05822928604225119</v>
+        <v>-0.203341095319014</v>
       </c>
       <c r="I41">
-        <v>2.818293798261426</v>
+        <v>2.760850900332427</v>
       </c>
     </row>
     <row r="42">
@@ -1742,19 +1742,19 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>2.389424258125911</v>
+        <v>2.586131763444331</v>
       </c>
       <c r="F42">
-        <v>2.878932472238359</v>
+        <v>3.082359609215559</v>
       </c>
       <c r="G42">
-        <v>0.4845979988347779</v>
+        <v>0.4126589437105712</v>
       </c>
       <c r="H42">
-        <v>-0.5699963271677637</v>
+        <v>-0.2529313794777771</v>
       </c>
       <c r="I42">
-        <v>2.474822586458897</v>
+        <v>2.426404199211537</v>
       </c>
     </row>
     <row r="43">
@@ -1775,19 +1775,19 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1.55853274838479</v>
+        <v>1.766412190866032</v>
       </c>
       <c r="F43">
-        <v>2.395579232947894</v>
+        <v>2.596883992470003</v>
       </c>
       <c r="G43">
-        <v>0.6580666105653628</v>
+        <v>-0.003475118545377909</v>
       </c>
       <c r="H43">
-        <v>-1.231557517884624</v>
+        <v>-0.3262867692559824</v>
       </c>
       <c r="I43">
-        <v>2.132023655704051</v>
+        <v>2.096174078667393</v>
       </c>
     </row>
     <row r="44">
@@ -1808,19 +1808,19 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>1.197155146805813</v>
+        <v>1.423722709723258</v>
       </c>
       <c r="F44">
-        <v>1.984695653403127</v>
+        <v>2.191303238811282</v>
       </c>
       <c r="G44">
-        <v>0.3629357418181439</v>
+        <v>0.4217013248878961</v>
       </c>
       <c r="H44">
-        <v>-0.3190249714830934</v>
+        <v>-0.1268230767511501</v>
       </c>
       <c r="I44">
-        <v>1.153244376470763</v>
+        <v>1.128844461586512</v>
       </c>
     </row>
     <row r="45">
@@ -1841,19 +1841,19 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0.2537911406297905</v>
+        <v>0.5026285094021906</v>
       </c>
       <c r="F45">
-        <v>1.349725823486575</v>
+        <v>1.569723793358952</v>
       </c>
       <c r="G45">
-        <v>0.3217281103194144</v>
+        <v>-0.7703781740154796</v>
       </c>
       <c r="H45">
-        <v>-1.163869244352827</v>
+        <v>0.1901146834763395</v>
       </c>
       <c r="I45">
-        <v>1.095932274663203</v>
+        <v>1.082891999941331</v>
       </c>
     </row>
     <row r="46">
@@ -1874,19 +1874,19 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.2213946766142565</v>
+        <v>0.4873346297696639</v>
       </c>
       <c r="F46">
-        <v>0.807718428108661</v>
+        <v>1.045024509940285</v>
       </c>
       <c r="G46">
-        <v>-0.4301179829136424</v>
+        <v>0.1696321872222053</v>
       </c>
       <c r="H46">
-        <v>-0.3645417463103539</v>
+        <v>-0.696185701270406</v>
       </c>
       <c r="I46">
-        <v>1.016054405838253</v>
+        <v>1.013888143817865</v>
       </c>
     </row>
     <row r="47">
@@ -1907,19 +1907,19 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>-1.512403547515539</v>
+        <v>-1.227882409573331</v>
       </c>
       <c r="F47">
-        <v>0.03998435413357859</v>
+        <v>0.2964508598304444</v>
       </c>
       <c r="G47">
-        <v>-1.290592185633025</v>
+        <v>0.1684697069789879</v>
       </c>
       <c r="H47">
-        <v>-0.009319673892661418</v>
+        <v>-1.191274748505505</v>
       </c>
       <c r="I47">
-        <v>-0.2124916879898528</v>
+        <v>-0.2050773680468146</v>
       </c>
     </row>
     <row r="48">
@@ -1940,19 +1940,19 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>-1.329008622253417</v>
+        <v>-1.033731099293842</v>
       </c>
       <c r="F48">
-        <v>-0.5915565881312289</v>
+        <v>-0.3179125924238306</v>
       </c>
       <c r="G48">
-        <v>-0.4342612224775001</v>
+        <v>0.01859064452557019</v>
       </c>
       <c r="H48">
-        <v>-0.4135894254409594</v>
+        <v>-0.5812383154098705</v>
       </c>
       <c r="I48">
-        <v>-0.4811579743349573</v>
+        <v>-0.4710834284095413</v>
       </c>
     </row>
     <row r="49">
@@ -1973,19 +1973,19 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>-2.147976703534926</v>
+        <v>-1.843362313228648</v>
       </c>
       <c r="F49">
-        <v>-1.191998549172408</v>
+        <v>-0.9044102980815402</v>
       </c>
       <c r="G49">
-        <v>-2.482048414043194</v>
+        <v>0.844913545254637</v>
       </c>
       <c r="H49">
-        <v>1.020447248806644</v>
+        <v>-2.013634932113948</v>
       </c>
       <c r="I49">
-        <v>-0.6863755382983762</v>
+        <v>-0.6746409263693368</v>
       </c>
     </row>
     <row r="50">
@@ -2006,19 +2006,19 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>-1.097164219896707</v>
+        <v>-0.7919320487585149</v>
       </c>
       <c r="F50">
-        <v>-1.521638273300149</v>
+        <v>-1.224226967713585</v>
       </c>
       <c r="G50">
-        <v>-0.1717916821740831</v>
+        <v>0.2562045734879467</v>
       </c>
       <c r="H50">
-        <v>-0.1791952410126122</v>
+        <v>-0.3122102720358756</v>
       </c>
       <c r="I50">
-        <v>-0.7461772967100115</v>
+        <v>-0.7359263502105858</v>
       </c>
     </row>
     <row r="51">
@@ -2039,19 +2039,19 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>-1.474176269031964</v>
+        <v>-1.169471359151141</v>
       </c>
       <c r="F51">
-        <v>-1.512081453679255</v>
+        <v>-1.209624205108037</v>
       </c>
       <c r="G51">
-        <v>-0.3180207284257634</v>
+        <v>0.1450182149398946</v>
       </c>
       <c r="H51">
-        <v>-0.3289264061312071</v>
+        <v>-0.4947906108575231</v>
       </c>
       <c r="I51">
-        <v>-0.8272291344749938</v>
+        <v>-0.8196989632335121</v>
       </c>
     </row>
     <row r="52">
@@ -2072,19 +2072,19 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>-1.270989307518339</v>
+        <v>-0.9647842422069379</v>
       </c>
       <c r="F52">
-        <v>-1.497576624995486</v>
+        <v>-1.192387490836311</v>
       </c>
       <c r="G52">
-        <v>-0.2555011342392</v>
+        <v>-0.4323678523936096</v>
       </c>
       <c r="H52">
-        <v>-0.455113063631259</v>
+        <v>0.02432447663671006</v>
       </c>
       <c r="I52">
-        <v>-0.5603751096478804</v>
+        <v>-0.5567408664500384</v>
       </c>
     </row>
     <row r="53">
@@ -2105,19 +2105,19 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>-0.850115433964387</v>
+        <v>-0.5445147774382127</v>
       </c>
       <c r="F53">
-        <v>-1.173111307602851</v>
+        <v>-0.8676756068887025</v>
       </c>
       <c r="G53">
-        <v>-0.4271255494308367</v>
+        <v>0.3803818637273209</v>
       </c>
       <c r="H53">
-        <v>0.001119773954048608</v>
+        <v>-0.5017904711965351</v>
       </c>
       <c r="I53">
-        <v>-0.4241096584875989</v>
+        <v>-0.4231061699689986</v>
       </c>
     </row>
     <row r="54">
@@ -2138,19 +2138,19 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>-1.577666199735684</v>
+        <v>-1.269972864436758</v>
       </c>
       <c r="F54">
-        <v>-1.293236802562595</v>
+        <v>-0.9871858108082634</v>
       </c>
       <c r="G54">
-        <v>-0.7783775454409716</v>
+        <v>-0.6673024455224547</v>
       </c>
       <c r="H54">
-        <v>-0.2914504831101449</v>
+        <v>-0.09428784992988173</v>
       </c>
       <c r="I54">
-        <v>-0.5078381711845673</v>
+        <v>-0.5083825689844217</v>
       </c>
     </row>
     <row r="55">
@@ -2171,19 +2171,19 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>-1.807283111565523</v>
+        <v>-1.501064742175452</v>
       </c>
       <c r="F55">
-        <v>-1.376513513195984</v>
+        <v>-1.070084156564341</v>
       </c>
       <c r="G55">
-        <v>-1.179505110082348</v>
+        <v>-0.4174472957211435</v>
       </c>
       <c r="H55">
-        <v>0.1812511873214944</v>
+        <v>-0.2709188102602541</v>
       </c>
       <c r="I55">
-        <v>-0.8090291888046688</v>
+        <v>-0.8126986361940544</v>
       </c>
     </row>
     <row r="56">
@@ -2204,19 +2204,19 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>-1.296894900430044</v>
+        <v>-0.9938909145198351</v>
       </c>
       <c r="F56">
-        <v>-1.382989911423911</v>
+        <v>-1.077360824642565</v>
       </c>
       <c r="G56">
-        <v>-0.1060223784321607</v>
+        <v>-0.5559174319186626</v>
       </c>
       <c r="H56">
-        <v>-0.3377649070276527</v>
+        <v>0.4227614915339761</v>
       </c>
       <c r="I56">
-        <v>-0.8531076149702307</v>
+        <v>-0.8607349741351487</v>
       </c>
     </row>
     <row r="57">
@@ -2237,19 +2237,19 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>-1.147544433772517</v>
+        <v>-0.8478039753984121</v>
       </c>
       <c r="F57">
-        <v>-1.457347161375943</v>
+        <v>-1.153183124132615</v>
       </c>
       <c r="G57">
-        <v>-0.7339913447596539</v>
+        <v>-0.2997224000918609</v>
       </c>
       <c r="H57">
-        <v>0.01788900427050041</v>
+        <v>-0.1045155710692038</v>
       </c>
       <c r="I57">
-        <v>-0.4314420932833635</v>
+        <v>-0.4435660042373474</v>
       </c>
     </row>
     <row r="58">
@@ -2270,19 +2270,19 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>-1.391699613015229</v>
+        <v>-1.094792937704148</v>
       </c>
       <c r="F58">
-        <v>-1.410855514695829</v>
+        <v>-1.109388142449462</v>
       </c>
       <c r="G58">
-        <v>-0.9610588632034938</v>
+        <v>-0.2240111183472178</v>
       </c>
       <c r="H58">
-        <v>0.05917737106952187</v>
+        <v>-0.3661740621074557</v>
       </c>
       <c r="I58">
-        <v>-0.4898181208812569</v>
+        <v>-0.5046077572494742</v>
       </c>
     </row>
     <row r="59">
@@ -2303,19 +2303,19 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>-1.281009764487658</v>
+        <v>-0.9874827118067558</v>
       </c>
       <c r="F59">
-        <v>-1.279287177926363</v>
+        <v>-0.9809926348572885</v>
       </c>
       <c r="G59">
-        <v>0.1673511113757621</v>
+        <v>-0.4061811825802247</v>
       </c>
       <c r="H59">
-        <v>-0.7890024496749073</v>
+        <v>0.0958164009158845</v>
       </c>
       <c r="I59">
-        <v>-0.6593584261885128</v>
+        <v>-0.6771179301424156</v>
       </c>
     </row>
     <row r="60">
@@ -2336,19 +2336,19 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>-0.7256627824444662</v>
+        <v>-0.4341834594629475</v>
       </c>
       <c r="F60">
-        <v>-1.136479148429969</v>
+        <v>-0.8410657710930665</v>
       </c>
       <c r="G60">
-        <v>0.2345572910757722</v>
+        <v>-0.7509726066732845</v>
       </c>
       <c r="H60">
-        <v>-0.4574747876149671</v>
+        <v>0.8413517740071288</v>
       </c>
       <c r="I60">
-        <v>-0.5027452859052713</v>
+        <v>-0.5245626267967918</v>
       </c>
     </row>
     <row r="61">
@@ -2369,19 +2369,19 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>-0.2214156928532106</v>
+        <v>0.06783137863381355</v>
       </c>
       <c r="F61">
-        <v>-0.9049469632001425</v>
+        <v>-0.61215693258501</v>
       </c>
       <c r="G61">
-        <v>0.5284396237065569</v>
+        <v>-0.0812099604090557</v>
       </c>
       <c r="H61">
-        <v>-0.3556249839539183</v>
+        <v>0.5670893333084116</v>
       </c>
       <c r="I61">
-        <v>-0.3942303326058492</v>
+        <v>-0.4180479942655423</v>
       </c>
     </row>
     <row r="62">
@@ -2402,19 +2402,19 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>-0.6018255286253917</v>
+        <v>-0.3146272822675598</v>
       </c>
       <c r="F62">
-        <v>-0.7074784421026832</v>
+        <v>-0.4171155187258631</v>
       </c>
       <c r="G62">
-        <v>-0.7998218326423571</v>
+        <v>-0.1957491219772411</v>
       </c>
       <c r="H62">
-        <v>0.4519125248281585</v>
+        <v>0.1610420819330972</v>
       </c>
       <c r="I62">
-        <v>-0.2539162208111932</v>
+        <v>-0.2799202422234159</v>
       </c>
     </row>
     <row r="63">
@@ -2435,19 +2435,19 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0.07567012183325031</v>
+        <v>0.3584729986892405</v>
       </c>
       <c r="F63">
-        <v>-0.3683084705224561</v>
+        <v>-0.08062659110186396</v>
       </c>
       <c r="G63">
-        <v>0.4638598756655173</v>
+        <v>-0.4074660776168579</v>
       </c>
       <c r="H63">
-        <v>-0.4070882279280646</v>
+        <v>0.7737859440606548</v>
       </c>
       <c r="I63">
-        <v>0.01889847409579756</v>
+        <v>-0.00784686775455639</v>
       </c>
     </row>
     <row r="64">
@@ -2468,19 +2468,19 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0.2955907407600904</v>
+        <v>0.5757686474308995</v>
       </c>
       <c r="F64">
-        <v>-0.112995089721317</v>
+        <v>0.1718614356215978</v>
       </c>
       <c r="G64">
-        <v>-0.1322437700437326</v>
+        <v>0.06277798709953475</v>
       </c>
       <c r="H64">
-        <v>0.4305159871690014</v>
+        <v>0.5420811257918118</v>
       </c>
       <c r="I64">
-        <v>-0.00268147636517846</v>
+        <v>-0.02909046546044699</v>
       </c>
     </row>
     <row r="65">
@@ -2501,19 +2501,19 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0.03570034961818545</v>
+        <v>0.3109781957376174</v>
       </c>
       <c r="F65">
-        <v>-0.04871607910346795</v>
+        <v>0.2326481398975487</v>
       </c>
       <c r="G65">
-        <v>-0.09137153200886633</v>
+        <v>-0.1327573957763631</v>
       </c>
       <c r="H65">
-        <v>0.1068756109715456</v>
+        <v>0.4514429786931769</v>
       </c>
       <c r="I65">
-        <v>0.02019627065550618</v>
+        <v>-0.007707387179196396</v>
       </c>
     </row>
     <row r="66">
@@ -2534,19 +2534,19 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>-0.1038810534372324</v>
+        <v>0.1654900310043851</v>
       </c>
       <c r="F66">
-        <v>0.07577003969357188</v>
+        <v>0.3526774682155349</v>
       </c>
       <c r="G66">
-        <v>0.4189975841590008</v>
+        <v>-0.1801940834457704</v>
       </c>
       <c r="H66">
-        <v>-0.4624177595199218</v>
+        <v>0.4351408046902969</v>
       </c>
       <c r="I66">
-        <v>-0.06046087807631146</v>
+        <v>-0.0894566902401415</v>
       </c>
     </row>
     <row r="67">
@@ -2567,19 +2567,19 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>0.3150678201718904</v>
+        <v>0.5805545259320211</v>
       </c>
       <c r="F67">
-        <v>0.1356194642782319</v>
+        <v>0.40819785002623</v>
       </c>
       <c r="G67">
-        <v>-0.1294776262718526</v>
+        <v>0.1446360764488608</v>
       </c>
       <c r="H67">
-        <v>0.4818270841889017</v>
+        <v>0.5046954554173962</v>
       </c>
       <c r="I67">
-        <v>-0.03728163774515877</v>
+        <v>-0.06877700593423601</v>
       </c>
     </row>
     <row r="68">
@@ -2600,19 +2600,19 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>-0.4750874140947117</v>
+        <v>-0.2198759278013104</v>
       </c>
       <c r="F68">
-        <v>-0.05705007443546861</v>
+        <v>0.2092867062181776</v>
       </c>
       <c r="G68">
-        <v>-0.1771022445143513</v>
+        <v>-0.3900965921543058</v>
       </c>
       <c r="H68">
-        <v>-0.2237848417004576</v>
+        <v>0.2771373206810341</v>
       </c>
       <c r="I68">
-        <v>-0.07420032787990281</v>
+        <v>-0.1069166563280386</v>
       </c>
     </row>
     <row r="69">
@@ -2633,19 +2633,19 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>-0.09131664228255593</v>
+        <v>0.1589285996046639</v>
       </c>
       <c r="F69">
-        <v>-0.08880432241065396</v>
+        <v>0.1712743071849392</v>
       </c>
       <c r="G69">
-        <v>0.1605813349989212</v>
+        <v>-0.08733488089964167</v>
       </c>
       <c r="H69">
-        <v>-0.1146050260107713</v>
+        <v>0.4167077288083179</v>
       </c>
       <c r="I69">
-        <v>-0.1372929512707058</v>
+        <v>-0.1704442483040124</v>
       </c>
     </row>
     <row r="70">
@@ -2666,19 +2666,19 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>-0.1995224324732995</v>
+        <v>0.04736046859605603</v>
       </c>
       <c r="F70">
-        <v>-0.1127146671696707</v>
+        <v>0.141741916582857</v>
       </c>
       <c r="G70">
-        <v>-0.01144993790299047</v>
+        <v>-0.1278436839455424</v>
       </c>
       <c r="H70">
-        <v>-0.08305788859239972</v>
+        <v>0.3139223053663386</v>
       </c>
       <c r="I70">
-        <v>-0.1050146059779094</v>
+        <v>-0.1387181528247401</v>
       </c>
     </row>
     <row r="71">
@@ -2699,19 +2699,19 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>-0.2124933417058218</v>
+        <v>0.03091987621313803</v>
       </c>
       <c r="F71">
-        <v>-0.2446049576390988</v>
+        <v>0.004333254153136207</v>
       </c>
       <c r="G71">
-        <v>-0.6394960957894104</v>
+        <v>0.2677292251719238</v>
       </c>
       <c r="H71">
-        <v>0.3662404479286187</v>
+        <v>-0.263229069689987</v>
       </c>
       <c r="I71">
-        <v>0.06076230615496983</v>
+        <v>0.02641972073120126</v>
       </c>
     </row>
     <row r="72">
@@ -2732,19 +2732,19 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0.06999808627090098</v>
+        <v>0.3181970772686439</v>
       </c>
       <c r="F72">
-        <v>-0.1083335825476956</v>
+        <v>0.1388515054206248</v>
       </c>
       <c r="G72">
-        <v>-0.4004341217725897</v>
+        <v>0.52312767676769</v>
       </c>
       <c r="H72">
-        <v>0.3876720798290918</v>
+        <v>-0.2543557166457277</v>
       </c>
       <c r="I72">
-        <v>0.08276012821439893</v>
+        <v>0.0494251171466816</v>
       </c>
     </row>
     <row r="73">
@@ -2765,19 +2765,19 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>-0.2322422349336884</v>
+        <v>0.02715540074993463</v>
       </c>
       <c r="F73">
-        <v>-0.1435649807104787</v>
+        <v>0.1059082057069425</v>
       </c>
       <c r="G73">
-        <v>0.01996843340862331</v>
+        <v>-0.2462085424130513</v>
       </c>
       <c r="H73">
-        <v>-0.2756000615749862</v>
+        <v>0.2811655584663052</v>
       </c>
       <c r="I73">
-        <v>0.02338939323267457</v>
+        <v>-0.007801615303319276</v>
       </c>
     </row>
     <row r="74">
@@ -2798,19 +2798,19 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0.03573077816420434</v>
+        <v>0.3033443014736101</v>
       </c>
       <c r="F74">
-        <v>-0.08475167805110277</v>
+        <v>0.169904163926331</v>
       </c>
       <c r="G74">
-        <v>0.2143447422167435</v>
+        <v>0.2626719596059693</v>
       </c>
       <c r="H74">
-        <v>-0.01771226396712674</v>
+        <v>0.2304793770639839</v>
       </c>
       <c r="I74">
-        <v>-0.1609017000854124</v>
+        <v>-0.1898070351963431</v>
       </c>
     </row>
     <row r="75">
@@ -2831,19 +2831,19 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0.01710185813511347</v>
+        <v>0.2946929863620202</v>
       </c>
       <c r="F75">
-        <v>-0.02735287809086894</v>
+        <v>0.2358474414635515</v>
       </c>
       <c r="G75">
-        <v>-0.009406648181136543</v>
+        <v>0.08774199681802211</v>
       </c>
       <c r="H75">
-        <v>-0.04207515758740355</v>
+        <v>0.1651340442225374</v>
       </c>
       <c r="I75">
-        <v>0.06858366390365357</v>
+        <v>0.04181694532146071</v>
       </c>
     </row>
     <row r="76">
@@ -2864,19 +2864,19 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0.4267561736687195</v>
+        <v>0.7150212350301939</v>
       </c>
       <c r="F76">
-        <v>0.06183664375858569</v>
+        <v>0.3350534809039389</v>
       </c>
       <c r="G76">
-        <v>-0.1487830137347019</v>
+        <v>0.4297577362167462</v>
       </c>
       <c r="H76">
-        <v>0.3385548399268041</v>
+        <v>0.07225776655800209</v>
       </c>
       <c r="I76">
-        <v>0.2369843474766172</v>
+        <v>0.2130057322554456</v>
       </c>
     </row>
     <row r="77">
@@ -2897,19 +2897,19 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0.1609137213607248</v>
+        <v>0.459101437449597</v>
       </c>
       <c r="F77">
-        <v>0.160125632832189</v>
+        <v>0.4430399900788545</v>
       </c>
       <c r="G77">
-        <v>0.1873374336061686</v>
+        <v>0.2109924963445054</v>
       </c>
       <c r="H77">
-        <v>-0.06964884868718382</v>
+        <v>0.226214317730833</v>
       </c>
       <c r="I77">
-        <v>0.04322513644174007</v>
+        <v>0.02189462337425864</v>
       </c>
     </row>
     <row r="78">
@@ -2930,19 +2930,19 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>-0.4160248471714142</v>
+        <v>-0.1145111792091212</v>
       </c>
       <c r="F78">
-        <v>0.04718672649828434</v>
+        <v>0.3385761199081717</v>
       </c>
       <c r="G78">
-        <v>-0.166406556291452</v>
+        <v>0.237122930151244</v>
       </c>
       <c r="H78">
-        <v>-0.3128533800933186</v>
+        <v>-0.3937263151375531</v>
       </c>
       <c r="I78">
-        <v>0.06323508921335651</v>
+        <v>0.04209220577718782</v>
       </c>
     </row>
     <row r="79">
@@ -2963,19 +2963,19 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0.210032098634459</v>
+        <v>0.5100233330183411</v>
       </c>
       <c r="F79">
-        <v>0.09541928662312071</v>
+        <v>0.392408706572252</v>
       </c>
       <c r="G79">
-        <v>0.1505743433155476</v>
+        <v>-0.1472996337848166</v>
       </c>
       <c r="H79">
-        <v>-0.04178406947945221</v>
+        <v>0.5780486871037616</v>
       </c>
       <c r="I79">
-        <v>0.1012418247983636</v>
+        <v>0.07927427969939616</v>
       </c>
     </row>
     <row r="80">
@@ -2996,19 +2996,19 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>0.6053860752659407</v>
+        <v>0.9039313416023554</v>
       </c>
       <c r="F80">
-        <v>0.140076762022426</v>
+        <v>0.4396362332152924</v>
       </c>
       <c r="G80">
-        <v>0.6286392149233443</v>
+        <v>0.3571800727378065</v>
       </c>
       <c r="H80">
-        <v>-0.08996722349663627</v>
+        <v>0.502883685661647</v>
       </c>
       <c r="I80">
-        <v>0.06671408383923272</v>
+        <v>0.04386758320290196</v>
       </c>
     </row>
     <row r="81">
@@ -3029,19 +3029,19 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>0.4166339228374313</v>
+        <v>0.7130827088832501</v>
       </c>
       <c r="F81">
-        <v>0.2040068123916027</v>
+        <v>0.5031315510737057</v>
       </c>
       <c r="G81">
-        <v>0.09592883154151852</v>
+        <v>0.3494500224676224</v>
       </c>
       <c r="H81">
-        <v>-0.04337606113221329</v>
+        <v>0.02425579270840394</v>
       </c>
       <c r="I81">
-        <v>0.3640811524281261</v>
+        <v>0.3393768937072238</v>
       </c>
     </row>
     <row r="82">
@@ -3062,19 +3062,19 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <v>0.4929232289815144</v>
+        <v>0.7860437779826436</v>
       </c>
       <c r="F82">
-        <v>0.4312438314298348</v>
+        <v>0.7282702903716468</v>
       </c>
       <c r="G82">
-        <v>0.1270173704331562</v>
+        <v>0.212703570123558</v>
       </c>
       <c r="H82">
-        <v>-0.03000270441402829</v>
+        <v>0.2037445872558542</v>
       </c>
       <c r="I82">
-        <v>0.3959085629623865</v>
+        <v>0.3695956206032314</v>
       </c>
     </row>
     <row r="83">
@@ -3095,19 +3095,19 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>0.06261001664075963</v>
+        <v>0.354734714897042</v>
       </c>
       <c r="F83">
-        <v>0.39438831093141</v>
+        <v>0.689448135841322</v>
       </c>
       <c r="G83">
-        <v>0.09925778107690075</v>
+        <v>-0.067915184401038</v>
       </c>
       <c r="H83">
-        <v>-0.1952725638729471</v>
+        <v>0.2893119225244437</v>
       </c>
       <c r="I83">
-        <v>0.1586247994368059</v>
+        <v>0.1333379767736363</v>
       </c>
     </row>
     <row r="84">
@@ -3128,19 +3128,19 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>14.09331751868514</v>
+        <v>14.38823221072811</v>
       </c>
       <c r="F84">
-        <v>3.766371171786211</v>
+        <v>4.06052335312276</v>
       </c>
       <c r="G84">
-        <v>-5.517447705263546</v>
+        <v>-13.31659129694795</v>
       </c>
       <c r="H84">
-        <v>5.63089391030197</v>
+        <v>13.75712049673779</v>
       </c>
       <c r="I84">
-        <v>13.97987131364672</v>
+        <v>13.94770301093826</v>
       </c>
     </row>
     <row r="85">
@@ -3161,19 +3161,19 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>5.413203250731433</v>
+        <v>5.68753667964231</v>
       </c>
       <c r="F85">
-        <v>5.015513503759712</v>
+        <v>5.304136845812526</v>
       </c>
       <c r="G85">
-        <v>-0.5073236800666964</v>
+        <v>13.49528513621632</v>
       </c>
       <c r="H85">
-        <v>-0.6537520414966955</v>
+        <v>-14.39457650423646</v>
       </c>
       <c r="I85">
-        <v>6.574278972294826</v>
+        <v>6.586828047662447</v>
       </c>
     </row>
     <row r="86">
@@ -3191,19 +3191,19 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <v>-1.166489776668105</v>
+        <v>2.35726868646428</v>
       </c>
       <c r="F86">
-        <v>4.600660252347307</v>
+        <v>5.696943072932934</v>
       </c>
       <c r="G86">
-        <v>9.741032883434654</v>
+        <v>0.04857539883383277</v>
       </c>
       <c r="H86">
-        <v>-9.908519894775949</v>
+        <v>0.02072997815986104</v>
       </c>
       <c r="I86">
-        <v>-0.9990027653268098</v>
+        <v>2.287963309470586</v>
       </c>
     </row>
     <row r="87">
@@ -3221,19 +3221,19 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>-0.721670403609916</v>
+        <v>2.280501568416709</v>
       </c>
       <c r="F87">
-        <v>4.404590147284638</v>
+        <v>6.178384786312852</v>
       </c>
       <c r="G87">
-        <v>-0.1504361214857687</v>
+        <v>-0.01027304119107209</v>
       </c>
       <c r="H87">
-        <v>-0.1186137767180931</v>
+        <v>-0.01755779857712431</v>
       </c>
       <c r="I87">
-        <v>-0.4526205054060542</v>
+        <v>2.308332408184905</v>
       </c>
     </row>
     <row r="88">
@@ -3251,19 +3251,19 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>-7.211003012333482</v>
+        <v>-4.956896080158649</v>
       </c>
       <c r="F88">
-        <v>-0.9214899854700187</v>
+        <v>1.342102713591162</v>
       </c>
       <c r="G88">
-        <v>-0.4226600391658379</v>
+        <v>-0.004597315773347131</v>
       </c>
       <c r="H88">
-        <v>0.004763862455765933</v>
+        <v>-0.1594263942033482</v>
       </c>
       <c r="I88">
-        <v>-6.793106835623409</v>
+        <v>-4.792872370181954</v>
       </c>
     </row>
     <row r="89">
@@ -3281,19 +3281,19 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>-4.191912019167354</v>
+        <v>-1.841703245042833</v>
       </c>
       <c r="F89">
-        <v>-3.322768802944716</v>
+        <v>-0.5402072675801235</v>
       </c>
       <c r="G89">
-        <v>0.1232010657046651</v>
+        <v>0.02170019548771828</v>
       </c>
       <c r="H89">
-        <v>-0.3994621873585893</v>
+        <v>-0.02817972998782436</v>
       </c>
       <c r="I89">
-        <v>-3.91565089751343</v>
+        <v>-1.835223710542727</v>
       </c>
     </row>
     <row r="90">
@@ -3311,19 +3311,19 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>-2.141011121978358</v>
+        <v>-0.5111454392783423</v>
       </c>
       <c r="F90">
-        <v>-3.566399139272279</v>
+        <v>-1.257310799015779</v>
       </c>
       <c r="G90">
-        <v>-0.3511588688039241</v>
+        <v>0.04918932641535643</v>
       </c>
       <c r="H90">
-        <v>0.2293869335764527</v>
+        <v>0.1154172155274835</v>
       </c>
       <c r="I90">
-        <v>-2.019239186750887</v>
+        <v>-0.6757519812211823</v>
       </c>
     </row>
     <row r="91">
@@ -3341,19 +3341,19 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>-1.058372831810453</v>
+        <v>0.7614199045831415</v>
       </c>
       <c r="F91">
-        <v>-3.650574746322413</v>
+        <v>-1.637081214974171</v>
       </c>
       <c r="G91">
-        <v>-0.350305360184503</v>
+        <v>0.06143017366114166</v>
       </c>
       <c r="H91">
-        <v>0.2933595027482839</v>
+        <v>0.1766350690546228</v>
       </c>
       <c r="I91">
-        <v>-1.001426974374234</v>
+        <v>0.523354661867377</v>
       </c>
     </row>
     <row r="92">
@@ -3371,19 +3371,19 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <v>-1.54178164695616</v>
+        <v>0.408557712088676</v>
       </c>
       <c r="F92">
-        <v>-2.233269404978083</v>
+        <v>-0.2957177669123399</v>
       </c>
       <c r="G92">
-        <v>-0.2492954117547802</v>
+        <v>0.06950155704309871</v>
       </c>
       <c r="H92">
-        <v>0.191835107665844</v>
+        <v>0.1714904397493573</v>
       </c>
       <c r="I92">
-        <v>-1.484321342867224</v>
+        <v>0.16756571529622</v>
       </c>
     </row>
     <row r="93">
@@ -3401,19 +3401,1009 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <v>-0.8083169949575513</v>
+        <v>1.186398798122388</v>
       </c>
       <c r="F93">
-        <v>-1.387370648925632</v>
+        <v>0.4613077438789654</v>
       </c>
       <c r="G93">
-        <v>-0.2254828502645548</v>
+        <v>0.08141126901291662</v>
       </c>
       <c r="H93">
-        <v>0.1298683800340012</v>
+        <v>0.123937594738118</v>
       </c>
       <c r="I93">
-        <v>-0.7127025247269977</v>
+        <v>0.9810499343713539</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1.018542800418538</v>
+      </c>
+      <c r="F94">
+        <v>0.8437298038031855</v>
+      </c>
+      <c r="G94">
+        <v>0.06935388160933978</v>
+      </c>
+      <c r="H94">
+        <v>0.05264139332557015</v>
+      </c>
+      <c r="I94">
+        <v>0.8965475254836279</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>0.9508742633159136</v>
+      </c>
+      <c r="F95">
+        <v>0.8910933934863786</v>
+      </c>
+      <c r="G95">
+        <v>0.08590903824618745</v>
+      </c>
+      <c r="H95">
+        <v>0.04778863170335976</v>
+      </c>
+      <c r="I95">
+        <v>0.8171765933663664</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>-0.2555452866529461</v>
+      </c>
+      <c r="F96">
+        <v>0.7250676438009731</v>
+      </c>
+      <c r="G96">
+        <v>0.07700983435727018</v>
+      </c>
+      <c r="H96">
+        <v>0.06528966948721746</v>
+      </c>
+      <c r="I96">
+        <v>-0.3978447904974338</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>-0.3619068036424422</v>
+      </c>
+      <c r="F97">
+        <v>0.3379912433597654</v>
+      </c>
+      <c r="G97">
+        <v>0.08623278322234249</v>
+      </c>
+      <c r="H97">
+        <v>0.06594634262832726</v>
+      </c>
+      <c r="I97">
+        <v>-0.5140859294931119</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>-0.3047430509294838</v>
+      </c>
+      <c r="F98">
+        <v>0.007169780522760016</v>
+      </c>
+      <c r="G98">
+        <v>0.08712163828799853</v>
+      </c>
+      <c r="H98">
+        <v>0.06320056879746458</v>
+      </c>
+      <c r="I98">
+        <v>-0.4550652580149469</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>-0.2339193026354872</v>
+      </c>
+      <c r="F99">
+        <v>-0.2890286109650902</v>
+      </c>
+      <c r="G99">
+        <v>0.08774731345951726</v>
+      </c>
+      <c r="H99">
+        <v>0.07407871035007121</v>
+      </c>
+      <c r="I99">
+        <v>-0.3957453264450757</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>-0.1764761964295454</v>
+      </c>
+      <c r="F100">
+        <v>-0.26926133840924</v>
+      </c>
+      <c r="G100">
+        <v>0.09210876307094044</v>
+      </c>
+      <c r="H100">
+        <v>0.08775627135805916</v>
+      </c>
+      <c r="I100">
+        <v>-0.356341230858545</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>-0.1241318607872378</v>
+      </c>
+      <c r="F101">
+        <v>-0.2098176026954389</v>
+      </c>
+      <c r="G101">
+        <v>0.09057717868205284</v>
+      </c>
+      <c r="H101">
+        <v>0.1044977439872774</v>
+      </c>
+      <c r="I101">
+        <v>-0.3192067834565681</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>0.08200207810420825</v>
+      </c>
+      <c r="F102">
+        <v>-0.1131313204370159</v>
+      </c>
+      <c r="G102">
+        <v>0.09186491527016931</v>
+      </c>
+      <c r="H102">
+        <v>0.1036308069896782</v>
+      </c>
+      <c r="I102">
+        <v>-0.1134936441556392</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>0.2572849758099054</v>
+      </c>
+      <c r="F103">
+        <v>0.009669749174332234</v>
+      </c>
+      <c r="G103">
+        <v>0.09929548036147109</v>
+      </c>
+      <c r="H103">
+        <v>0.1087313245447544</v>
+      </c>
+      <c r="I103">
+        <v>0.04925817090367997</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>0.3686276035911604</v>
+      </c>
+      <c r="F104">
+        <v>0.1459456991795087</v>
+      </c>
+      <c r="G104">
+        <v>0.08779439273809758</v>
+      </c>
+      <c r="H104">
+        <v>0.103696956913915</v>
+      </c>
+      <c r="I104">
+        <v>0.1771362539391478</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>0.4902674286120825</v>
+      </c>
+      <c r="F105">
+        <v>0.2995455215293388</v>
+      </c>
+      <c r="G105">
+        <v>0.08600867201388775</v>
+      </c>
+      <c r="H105">
+        <v>0.113067894768955</v>
+      </c>
+      <c r="I105">
+        <v>0.2911908618292398</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>0.3720943033812976</v>
+      </c>
+      <c r="F106">
+        <v>0.3720685778486111</v>
+      </c>
+      <c r="G106">
+        <v>0.08694914593174133</v>
+      </c>
+      <c r="H106">
+        <v>0.1174934804908915</v>
+      </c>
+      <c r="I106">
+        <v>0.1676516769586647</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>0.2369407208366761</v>
+      </c>
+      <c r="F107">
+        <v>0.3669825141053037</v>
+      </c>
+      <c r="G107">
+        <v>0.09401807708085538</v>
+      </c>
+      <c r="H107">
+        <v>0.1199903831794353</v>
+      </c>
+      <c r="I107">
+        <v>0.02293226057638545</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>0.1028740919827614</v>
+      </c>
+      <c r="F108">
+        <v>0.300544136203204</v>
+      </c>
+      <c r="G108">
+        <v>0.08404277736209484</v>
+      </c>
+      <c r="H108">
+        <v>0.1281157486980009</v>
+      </c>
+      <c r="I108">
+        <v>-0.1092844340773343</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>0.05054439716311382</v>
+      </c>
+      <c r="F109">
+        <v>0.1906133783409619</v>
+      </c>
+      <c r="G109">
+        <v>0.09372602752027656</v>
+      </c>
+      <c r="H109">
+        <v>0.1371685485380706</v>
+      </c>
+      <c r="I109">
+        <v>-0.1803501788952334</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>0.02536089178209511</v>
+      </c>
+      <c r="F110">
+        <v>0.1039300254411613</v>
+      </c>
+      <c r="G110">
+        <v>0.08288619960389453</v>
+      </c>
+      <c r="H110">
+        <v>0.1272834246426288</v>
+      </c>
+      <c r="I110">
+        <v>-0.1848087324644282</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2027</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>0.01480129171361555</v>
+      </c>
+      <c r="F111">
+        <v>0.04839516816039612</v>
+      </c>
+      <c r="G111">
+        <v>0.08114731743409459</v>
+      </c>
+      <c r="H111">
+        <v>0.1216355029039191</v>
+      </c>
+      <c r="I111">
+        <v>-0.1879815286243981</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2027</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>0.01483141214605652</v>
+      </c>
+      <c r="F112">
+        <v>0.02638449820121988</v>
+      </c>
+      <c r="G112">
+        <v>0.0903487970496613</v>
+      </c>
+      <c r="H112">
+        <v>0.1336220140862494</v>
+      </c>
+      <c r="I112">
+        <v>-0.2091393989898541</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2027</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>-0.04341839942418138</v>
+      </c>
+      <c r="F113">
+        <v>0.002893799054396084</v>
+      </c>
+      <c r="G113">
+        <v>0.08179600082270219</v>
+      </c>
+      <c r="H113">
+        <v>0.1159966362588275</v>
+      </c>
+      <c r="I113">
+        <v>-0.241211036505711</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2027</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>0.08938692880928215</v>
+      </c>
+      <c r="F114">
+        <v>0.01890030831119284</v>
+      </c>
+      <c r="G114">
+        <v>0.09158051193547388</v>
+      </c>
+      <c r="H114">
+        <v>0.1266296814582444</v>
+      </c>
+      <c r="I114">
+        <v>-0.1288232645844361</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>0.2474946718919476</v>
+      </c>
+      <c r="F115">
+        <v>0.07707365335577585</v>
+      </c>
+      <c r="G115">
+        <v>0.07789995006246449</v>
+      </c>
+      <c r="H115">
+        <v>0.1225515944132212</v>
+      </c>
+      <c r="I115">
+        <v>0.04704312741626194</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>0.4247653197147634</v>
+      </c>
+      <c r="F116">
+        <v>0.1795571302479526</v>
+      </c>
+      <c r="G116">
+        <v>0.08990201275527698</v>
+      </c>
+      <c r="H116">
+        <v>0.1240843062454546</v>
+      </c>
+      <c r="I116">
+        <v>0.2107790007140318</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>0.5430076217711095</v>
+      </c>
+      <c r="F117">
+        <v>0.3261636355467753</v>
+      </c>
+      <c r="G117">
+        <v>0.08760535940225586</v>
+      </c>
+      <c r="H117">
+        <v>0.1228872357935694</v>
+      </c>
+      <c r="I117">
+        <v>0.3325150265752842</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>0.1937638721227223</v>
+      </c>
+      <c r="F118">
+        <v>0.3522578713751354</v>
+      </c>
+      <c r="G118">
+        <v>0.081673190359142</v>
+      </c>
+      <c r="H118">
+        <v>0.1075013406551448</v>
+      </c>
+      <c r="I118">
+        <v>0.004589341108435545</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2029</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <v>-0.06842187696097701</v>
+      </c>
+      <c r="F119">
+        <v>0.2732787341619042</v>
+      </c>
+      <c r="G119">
+        <v>0.08748634379977589</v>
+      </c>
+      <c r="H119">
+        <v>0.1164891427276432</v>
+      </c>
+      <c r="I119">
+        <v>-0.2723973634883961</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2029</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>-0.3086553140299675</v>
+      </c>
+      <c r="F120">
+        <v>0.08992357572572152</v>
+      </c>
+      <c r="G120">
+        <v>0.0789423295887997</v>
+      </c>
+      <c r="H120">
+        <v>0.1032289546275242</v>
+      </c>
+      <c r="I120">
+        <v>-0.4908265982462914</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2029</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>-0.4623907632650178</v>
+      </c>
+      <c r="F121">
+        <v>-0.1614260205333103</v>
+      </c>
+      <c r="G121">
+        <v>0.08640582963345511</v>
+      </c>
+      <c r="H121">
+        <v>0.1054295879463654</v>
+      </c>
+      <c r="I121">
+        <v>-0.6542261808448383</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2029</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>-0.02570215768428852</v>
+      </c>
+      <c r="F122">
+        <v>-0.216292527985063</v>
+      </c>
+      <c r="G122">
+        <v>0.08433561844511164</v>
+      </c>
+      <c r="H122">
+        <v>0.1032730692030654</v>
+      </c>
+      <c r="I122">
+        <v>-0.2133108453324656</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>0.3008458145420495</v>
+      </c>
+      <c r="F123">
+        <v>-0.1239756051093064</v>
+      </c>
+      <c r="G123">
+        <v>0.07793576744425164</v>
+      </c>
+      <c r="H123">
+        <v>0.09159652837716471</v>
+      </c>
+      <c r="I123">
+        <v>0.1313135187206331</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>0.560918096246888</v>
+      </c>
+      <c r="F124">
+        <v>0.09341774745990751</v>
+      </c>
+      <c r="G124">
+        <v>0.08374160693595974</v>
+      </c>
+      <c r="H124">
+        <v>0.09145853608803493</v>
+      </c>
+      <c r="I124">
+        <v>0.3857179532228933</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>0.7395774443746777</v>
+      </c>
+      <c r="F125">
+        <v>0.3939097993698313</v>
+      </c>
+      <c r="G125">
+        <v>0.0861952988179496</v>
+      </c>
+      <c r="H125">
+        <v>0.08814783066061858</v>
+      </c>
+      <c r="I125">
+        <v>0.5652343148961094</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126">
+        <v>0.6158844132437238</v>
+      </c>
+      <c r="F126">
+        <v>0.5543064421018344</v>
+      </c>
+      <c r="G126">
+        <v>0.08048654268306082</v>
+      </c>
+      <c r="H126">
+        <v>0.08581514049466892</v>
+      </c>
+      <c r="I126">
+        <v>0.449582730065994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mpc's for unemployment insurance and rebate checks
</commit_message>
<xml_diff>
--- a/development/features/nipa-consistent-FIM/results/11-2020/data/fim_interactive.xlsx
+++ b/development/features/nipa-consistent-FIM/results/11-2020/data/fim_interactive.xlsx
@@ -422,10 +422,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.4866631286973806</v>
+        <v>0.4674476495037589</v>
       </c>
       <c r="F2">
-        <v>0.08145843961538593</v>
+        <v>0.07892722456184012</v>
       </c>
       <c r="G2">
         <v>0.4946888839019331</v>
@@ -434,7 +434,7 @@
         <v>0.6371181255487443</v>
       </c>
       <c r="I2">
-        <v>-0.6451438807532968</v>
+        <v>-0.6643593599469184</v>
       </c>
     </row>
     <row r="3">
@@ -455,10 +455,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-1.369571302537179</v>
+        <v>-1.368241615699741</v>
       </c>
       <c r="F3">
-        <v>-0.2203173382372797</v>
+        <v>-0.2235917018069998</v>
       </c>
       <c r="G3">
         <v>-0.6648250072254314</v>
@@ -467,7 +467,7 @@
         <v>0.1590883676069691</v>
       </c>
       <c r="I3">
-        <v>-0.8638346629187166</v>
+        <v>-0.8625049760812787</v>
       </c>
     </row>
     <row r="4">
@@ -488,10 +488,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1757862109959885</v>
+        <v>0.176989407323245</v>
       </c>
       <c r="F4">
-        <v>-0.0941847482093784</v>
+        <v>-0.1008613223178077</v>
       </c>
       <c r="G4">
         <v>0.7419382413465793</v>
@@ -500,7 +500,7 @@
         <v>-0.03911689401130113</v>
       </c>
       <c r="I4">
-        <v>-0.5270351363392897</v>
+        <v>-0.5258319400120331</v>
       </c>
     </row>
     <row r="5">
@@ -521,10 +521,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>-0.6476315805455177</v>
+        <v>-0.6518500158712432</v>
       </c>
       <c r="F5">
-        <v>-0.3386883858473326</v>
+        <v>-0.3439136436859948</v>
       </c>
       <c r="G5">
         <v>-0.8358291621042218</v>
@@ -533,7 +533,7 @@
         <v>0.5299153898310077</v>
       </c>
       <c r="I5">
-        <v>-0.3417178082723037</v>
+        <v>-0.3459362435980293</v>
       </c>
     </row>
     <row r="6">
@@ -554,10 +554,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.1985638843019602</v>
+        <v>0.2211723793194001</v>
       </c>
       <c r="F6">
-        <v>-0.4107131969461877</v>
+        <v>-0.4054824612320845</v>
       </c>
       <c r="G6">
         <v>-0.004798706463803183</v>
@@ -566,7 +566,7 @@
         <v>0.4375539874872086</v>
       </c>
       <c r="I6">
-        <v>-0.2341913967214452</v>
+        <v>-0.2115829017040053</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.082615219238455</v>
+        <v>1.154487130979547</v>
       </c>
       <c r="F7">
-        <v>0.2023334334977208</v>
+        <v>0.2251997254377376</v>
       </c>
       <c r="G7">
         <v>0.1167020212982178</v>
@@ -599,7 +599,7 @@
         <v>0.9814371046878589</v>
       </c>
       <c r="I7">
-        <v>-0.01552390674762178</v>
+        <v>0.05634800499347029</v>
       </c>
     </row>
     <row r="8">
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1.408990803744109</v>
+        <v>1.501643308236255</v>
       </c>
       <c r="F8">
-        <v>0.5106345816847511</v>
+        <v>0.55636320066599</v>
       </c>
       <c r="G8">
         <v>-0.005555307703252244</v>
@@ -632,7 +632,7 @@
         <v>1.277767859852481</v>
       </c>
       <c r="I8">
-        <v>0.1367782515948805</v>
+        <v>0.2294307560870256</v>
       </c>
     </row>
     <row r="9">
@@ -653,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1.183716102423204</v>
+        <v>1.289540135726599</v>
       </c>
       <c r="F9">
-        <v>0.9684715024269315</v>
+        <v>1.04171073856545</v>
       </c>
       <c r="G9">
         <v>0.3314497821167763</v>
@@ -665,7 +665,7 @@
         <v>-0.4053306945159103</v>
       </c>
       <c r="I9">
-        <v>1.257597014822338</v>
+        <v>1.363421048125733</v>
       </c>
     </row>
     <row r="10">
@@ -686,10 +686,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>2.221969928712494</v>
+        <v>2.402977599349805</v>
       </c>
       <c r="F10">
-        <v>1.474323013529565</v>
+        <v>1.587162043573052</v>
       </c>
       <c r="G10">
         <v>-0.1344040332508526</v>
@@ -698,7 +698,7 @@
         <v>1.355077793805707</v>
       </c>
       <c r="I10">
-        <v>1.001296168157639</v>
+        <v>1.182303838794951</v>
       </c>
     </row>
     <row r="11">
@@ -719,10 +719,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2.586814060087027</v>
+        <v>2.735814243523856</v>
       </c>
       <c r="F11">
-        <v>1.850372723741708</v>
+        <v>1.982493821709129</v>
       </c>
       <c r="G11">
         <v>0.3783184320669671</v>
@@ -731,7 +731,7 @@
         <v>0.9206418771130547</v>
       </c>
       <c r="I11">
-        <v>1.287853750907005</v>
+        <v>1.436853934343834</v>
       </c>
     </row>
     <row r="12">
@@ -752,10 +752,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2.219544332819797</v>
+        <v>2.512817068334928</v>
       </c>
       <c r="F12">
-        <v>2.05301110601063</v>
+        <v>2.235287261733798</v>
       </c>
       <c r="G12">
         <v>0.5148298247743641</v>
@@ -764,7 +764,7 @@
         <v>0.07245834106173334</v>
       </c>
       <c r="I12">
-        <v>1.6322561669837</v>
+        <v>1.92552890249883</v>
       </c>
     </row>
     <row r="13">
@@ -785,10 +785,10 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1.752047463842777</v>
+        <v>1.961289214139519</v>
       </c>
       <c r="F13">
-        <v>2.195093946365523</v>
+        <v>2.403224531337028</v>
       </c>
       <c r="G13">
         <v>0.1871948514362173</v>
@@ -797,7 +797,7 @@
         <v>0.2215417545996476</v>
       </c>
       <c r="I13">
-        <v>1.343310857806913</v>
+        <v>1.552552608103654</v>
       </c>
     </row>
     <row r="14">
@@ -818,10 +818,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1.620606130049476</v>
+        <v>1.520057027977812</v>
       </c>
       <c r="F14">
-        <v>2.044752996699768</v>
+        <v>2.18249438849403</v>
       </c>
       <c r="G14">
         <v>0.3438176679836201</v>
@@ -830,7 +830,7 @@
         <v>0.2552844291665327</v>
       </c>
       <c r="I14">
-        <v>1.021504032899323</v>
+        <v>0.920954930827659</v>
       </c>
     </row>
     <row r="15">
@@ -851,10 +851,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1.143308711697002</v>
+        <v>1.068606845725605</v>
       </c>
       <c r="F15">
-        <v>1.683876659602261</v>
+        <v>1.765692539044467</v>
       </c>
       <c r="G15">
         <v>0.4682780350108303</v>
@@ -863,7 +863,7 @@
         <v>-0.3784882380687687</v>
       </c>
       <c r="I15">
-        <v>1.05351891475494</v>
+        <v>0.9788170487835438</v>
       </c>
     </row>
     <row r="16">
@@ -884,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1.713066292210785</v>
+        <v>1.803727691141992</v>
       </c>
       <c r="F16">
-        <v>1.557257149450008</v>
+        <v>1.588420194746233</v>
       </c>
       <c r="G16">
         <v>-0.05414525130185377</v>
@@ -896,7 +896,7 @@
         <v>0.8001125511799414</v>
       </c>
       <c r="I16">
-        <v>0.967098992332697</v>
+        <v>1.057760391263905</v>
       </c>
     </row>
     <row r="17">
@@ -917,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.9220829822989938</v>
+        <v>1.003400899603621</v>
       </c>
       <c r="F17">
-        <v>1.349766029064062</v>
+        <v>1.348948116112259</v>
       </c>
       <c r="G17">
         <v>-0.0599874683905746</v>
@@ -929,7 +929,7 @@
         <v>0.2420652624995633</v>
       </c>
       <c r="I17">
-        <v>0.7400051881900052</v>
+        <v>0.8213231054946327</v>
       </c>
     </row>
     <row r="18">
@@ -950,10 +950,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1.081148290926134</v>
+        <v>0.9964378661507494</v>
       </c>
       <c r="F18">
-        <v>1.214901569283227</v>
+        <v>1.218043325655493</v>
       </c>
       <c r="G18">
         <v>0.5174208495565489</v>
@@ -962,7 +962,7 @@
         <v>-0.04216530301556628</v>
       </c>
       <c r="I18">
-        <v>0.6058927443851515</v>
+        <v>0.5211823196097668</v>
       </c>
     </row>
     <row r="19">
@@ -983,10 +983,10 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.5387853667922637</v>
+        <v>0.3449853342390917</v>
       </c>
       <c r="F19">
-        <v>1.063770733057043</v>
+        <v>1.037137947783865</v>
       </c>
       <c r="G19">
         <v>0.6358926447898382</v>
@@ -995,7 +995,7 @@
         <v>-0.2879900418715545</v>
       </c>
       <c r="I19">
-        <v>0.1908827638739801</v>
+        <v>-0.002917268679191926</v>
       </c>
     </row>
     <row r="20">
@@ -1016,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.3180383131787925</v>
+        <v>0.1061042097369443</v>
       </c>
       <c r="F20">
-        <v>0.7150137382990445</v>
+        <v>0.6127320774326032</v>
       </c>
       <c r="G20">
         <v>0.3082253456677642</v>
@@ -1028,7 +1028,7 @@
         <v>-0.09817299882337999</v>
       </c>
       <c r="I20">
-        <v>0.1079859663344083</v>
+        <v>-0.1039481371074398</v>
       </c>
     </row>
     <row r="21">
@@ -1049,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.08557310302885973</v>
+        <v>-0.1687725407114092</v>
       </c>
       <c r="F21">
-        <v>0.4630997169670811</v>
+        <v>0.3196887173538455</v>
       </c>
       <c r="G21">
         <v>0.4579664561789401</v>
@@ -1061,7 +1061,7 @@
         <v>-0.3143444540806857</v>
       </c>
       <c r="I21">
-        <v>-0.2291951051271141</v>
+        <v>-0.3123945428096636</v>
       </c>
     </row>
     <row r="22">
@@ -1082,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>-0.2637554299593816</v>
+        <v>-0.2982243612878771</v>
       </c>
       <c r="F22">
-        <v>0.1268737867457022</v>
+        <v>-0.003976839505811097</v>
       </c>
       <c r="G22">
         <v>-0.04764254032958169</v>
@@ -1094,7 +1094,7 @@
         <v>0.001415114232938797</v>
       </c>
       <c r="I22">
-        <v>-0.2175280038627387</v>
+        <v>-0.2519969351912342</v>
       </c>
     </row>
     <row r="23">
@@ -1115,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>-0.1924613699099915</v>
+        <v>-0.2569127064156363</v>
       </c>
       <c r="F23">
-        <v>-0.05593789742986166</v>
+        <v>-0.1544513496694931</v>
       </c>
       <c r="G23">
         <v>0.2259279932006186</v>
@@ -1127,7 +1127,7 @@
         <v>0.1608372538410204</v>
       </c>
       <c r="I23">
-        <v>-0.5792266169516305</v>
+        <v>-0.6436779534572753</v>
       </c>
     </row>
     <row r="24">
@@ -1148,10 +1148,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>-0.6101770594565787</v>
+        <v>-0.6815185059548368</v>
       </c>
       <c r="F24">
-        <v>-0.2879917405887045</v>
+        <v>-0.3513570285924384</v>
       </c>
       <c r="G24">
         <v>-0.01692944836407308</v>
@@ -1160,7 +1160,7 @@
         <v>-0.02771452247742881</v>
       </c>
       <c r="I24">
-        <v>-0.5655330886150768</v>
+        <v>-0.6368745351133348</v>
       </c>
     </row>
     <row r="25">
@@ -1181,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>-0.3502780325364347</v>
+        <v>-0.3813180362066679</v>
       </c>
       <c r="F25">
-        <v>-0.3541679729655982</v>
+        <v>-0.4044934024662531</v>
       </c>
       <c r="G25">
         <v>0.6052185045210049</v>
@@ -1193,7 +1193,7 @@
         <v>-0.3502867946894414</v>
       </c>
       <c r="I25">
-        <v>-0.6052097423679982</v>
+        <v>-0.6362497460382314</v>
       </c>
     </row>
     <row r="26">
@@ -1214,10 +1214,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>-0.4874592734445747</v>
+        <v>-0.4811124968434025</v>
       </c>
       <c r="F26">
-        <v>-0.4100939338368965</v>
+        <v>-0.4502154363551344</v>
       </c>
       <c r="G26">
         <v>0.0710785709364128</v>
@@ -1226,7 +1226,7 @@
         <v>-0.008790751509518233</v>
       </c>
       <c r="I26">
-        <v>-0.5497470928714693</v>
+        <v>-0.5434003162702971</v>
       </c>
     </row>
     <row r="27">
@@ -1247,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0.2626602897369307</v>
+        <v>0.2349163982107653</v>
       </c>
       <c r="F27">
-        <v>-0.2963135189251659</v>
+        <v>-0.3272581601985339</v>
       </c>
       <c r="G27">
         <v>0.864000865716967</v>
@@ -1259,7 +1259,7 @@
         <v>0.1069422092253407</v>
       </c>
       <c r="I27">
-        <v>-0.708282785205377</v>
+        <v>-0.7360266767315424</v>
       </c>
     </row>
     <row r="28">
@@ -1280,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>-0.7924740341364523</v>
+        <v>-0.8407142483349846</v>
       </c>
       <c r="F28">
-        <v>-0.3418877625951344</v>
+        <v>-0.3670570957935709</v>
       </c>
       <c r="G28">
         <v>-0.06876734097878898</v>
@@ -1292,7 +1292,7 @@
         <v>0.04683716166181404</v>
       </c>
       <c r="I28">
-        <v>-0.7705438548194774</v>
+        <v>-0.8187840690180097</v>
       </c>
     </row>
     <row r="29">
@@ -1313,10 +1313,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>-0.5118877722298127</v>
+        <v>-0.5141642137598463</v>
       </c>
       <c r="F29">
-        <v>-0.3822901975184789</v>
+        <v>-0.4002686401818655</v>
       </c>
       <c r="G29">
         <v>-0.3078566212245543</v>
@@ -1325,7 +1325,7 @@
         <v>0.1955365206213519</v>
       </c>
       <c r="I29">
-        <v>-0.3995676716266103</v>
+        <v>-0.4018441131566438</v>
       </c>
     </row>
     <row r="30">
@@ -1346,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.2042834843808807</v>
+        <v>0.2281766749913445</v>
       </c>
       <c r="F30">
-        <v>-0.209354508062115</v>
+        <v>-0.2229463472231788</v>
       </c>
       <c r="G30">
         <v>0.9226561346382511</v>
@@ -1358,7 +1358,7 @@
         <v>-0.2958138659857579</v>
       </c>
       <c r="I30">
-        <v>-0.4225587842716126</v>
+        <v>-0.3986655936611488</v>
       </c>
     </row>
     <row r="31">
@@ -1379,10 +1379,10 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>-0.337623163745105</v>
+        <v>-0.32498931423795</v>
       </c>
       <c r="F31">
-        <v>-0.359425371432624</v>
+        <v>-0.3629227753353576</v>
       </c>
       <c r="G31">
         <v>-0.6207245674312992</v>
@@ -1391,7 +1391,7 @@
         <v>0.732959001454615</v>
       </c>
       <c r="I31">
-        <v>-0.4498575977684208</v>
+        <v>-0.4372237482612658</v>
       </c>
     </row>
     <row r="32">
@@ -1412,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.331451106407301</v>
+        <v>0.3226338919222292</v>
       </c>
       <c r="F32">
-        <v>-0.07844408629668567</v>
+        <v>-0.07208574027105411</v>
       </c>
       <c r="G32">
         <v>0.418573520434026</v>
@@ -1424,7 +1424,7 @@
         <v>0.2797885772831269</v>
       </c>
       <c r="I32">
-        <v>-0.3669109913098519</v>
+        <v>-0.3757282057949236</v>
       </c>
     </row>
     <row r="33">
@@ -1445,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.2062588517926068</v>
+        <v>0.2047057271815161</v>
       </c>
       <c r="F33">
-        <v>0.1010925697089192</v>
+        <v>0.1076317449642865</v>
       </c>
       <c r="G33">
         <v>0.3870676995564565</v>
@@ -1457,7 +1457,7 @@
         <v>-0.03570683215632572</v>
       </c>
       <c r="I33">
-        <v>-0.145102015607524</v>
+        <v>-0.1466551402186148</v>
       </c>
     </row>
     <row r="34">
@@ -1478,10 +1478,10 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0.5468353249514979</v>
+        <v>0.5691530783848173</v>
       </c>
       <c r="F34">
-        <v>0.1867305298515735</v>
+        <v>0.1928758458126547</v>
       </c>
       <c r="G34">
         <v>0.7074003985694142</v>
@@ -1490,7 +1490,7 @@
         <v>-0.09925456184085245</v>
       </c>
       <c r="I34">
-        <v>-0.06131051177706377</v>
+        <v>-0.03899275834374435</v>
       </c>
     </row>
     <row r="35">
@@ -1511,10 +1511,10 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0.1900764248435546</v>
+        <v>0.2254993139496395</v>
       </c>
       <c r="F35">
-        <v>0.3186554269987384</v>
+        <v>0.3304980028595521</v>
       </c>
       <c r="G35">
         <v>0.3997191853271509</v>
@@ -1523,7 +1523,7 @@
         <v>-0.2220240185508833</v>
       </c>
       <c r="I35">
-        <v>0.012381258067287</v>
+        <v>0.04780414717337191</v>
       </c>
     </row>
     <row r="36">
@@ -1544,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>2.845147101950549</v>
+        <v>2.882573839860801</v>
       </c>
       <c r="F36">
-        <v>0.9470794258845505</v>
+        <v>0.9704829898441951</v>
       </c>
       <c r="G36">
         <v>0.5995147324770616</v>
@@ -1556,7 +1556,7 @@
         <v>0.08448158673897618</v>
       </c>
       <c r="I36">
-        <v>2.161150782734512</v>
+        <v>2.198577520644764</v>
       </c>
     </row>
     <row r="37">
@@ -1577,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1.609648225999502</v>
+        <v>1.837483157741453</v>
       </c>
       <c r="F37">
-        <v>1.297926769436274</v>
+        <v>1.378677347484179</v>
       </c>
       <c r="G37">
         <v>0.6723462386505684</v>
@@ -1589,7 +1589,7 @@
         <v>-0.03445495981190488</v>
       </c>
       <c r="I37">
-        <v>0.9717569471608384</v>
+        <v>1.199591878902789</v>
       </c>
     </row>
     <row r="38">
@@ -1610,10 +1610,10 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>1.786242053840766</v>
+        <v>2.159287518357699</v>
       </c>
       <c r="F38">
-        <v>1.607778451658591</v>
+        <v>1.7762109574774</v>
       </c>
       <c r="G38">
         <v>-0.06298272824822171</v>
@@ -1622,7 +1622,7 @@
         <v>0.592144784436984</v>
       </c>
       <c r="I38">
-        <v>1.257079997652004</v>
+        <v>1.630125462168937</v>
       </c>
     </row>
     <row r="39">
@@ -1643,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>3.708248798918394</v>
+        <v>4.18669070023828</v>
       </c>
       <c r="F39">
-        <v>2.487321545177301</v>
+        <v>2.76650880404956</v>
       </c>
       <c r="G39">
         <v>-0.9401670276868019</v>
@@ -1655,7 +1655,7 @@
         <v>1.84289552569623</v>
       </c>
       <c r="I39">
-        <v>2.805520300908966</v>
+        <v>3.283962202228853</v>
       </c>
     </row>
     <row r="40">
@@ -1676,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>3.045624961540685</v>
+        <v>3.66870452575498</v>
       </c>
       <c r="F40">
-        <v>2.537441010074835</v>
+        <v>2.963041475523105</v>
       </c>
       <c r="G40">
         <v>-0.6923124432083195</v>
@@ -1688,7 +1688,7 @@
         <v>1.895108765228772</v>
       </c>
       <c r="I40">
-        <v>1.842828639520233</v>
+        <v>2.465908203734527</v>
       </c>
     </row>
     <row r="41">
@@ -1709,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2.988764553142395</v>
+        <v>3.453474058076883</v>
       </c>
       <c r="F41">
-        <v>2.882220091860558</v>
+        <v>3.367039200606962</v>
       </c>
       <c r="G41">
         <v>0.4314364861980995</v>
@@ -1721,7 +1721,7 @@
         <v>-0.203341095319014</v>
       </c>
       <c r="I41">
-        <v>2.760669162263309</v>
+        <v>3.225378667197798</v>
       </c>
     </row>
     <row r="42">
@@ -1742,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>2.585965114092655</v>
+        <v>2.781348420175075</v>
       </c>
       <c r="F42">
-        <v>3.08215085692353</v>
+        <v>3.522554426061306</v>
       </c>
       <c r="G42">
         <v>0.4126589437105712</v>
@@ -1754,7 +1754,7 @@
         <v>-0.2529313794777771</v>
       </c>
       <c r="I42">
-        <v>2.426237549859861</v>
+        <v>2.621620855942281</v>
       </c>
     </row>
     <row r="43">
@@ -1775,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1.765547413409965</v>
+        <v>1.971580790638632</v>
       </c>
       <c r="F43">
-        <v>2.596475510546423</v>
+        <v>2.968776948661394</v>
       </c>
       <c r="G43">
         <v>-0.003475118545377909</v>
@@ -1787,7 +1787,7 @@
         <v>-0.3262867692559824</v>
       </c>
       <c r="I43">
-        <v>2.095309301211325</v>
+        <v>2.301342678439993</v>
       </c>
     </row>
     <row r="44">
@@ -1808,10 +1808,10 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>1.423972704509667</v>
+        <v>1.45780570175326</v>
       </c>
       <c r="F44">
-        <v>2.191062446288668</v>
+        <v>2.416052242660964</v>
       </c>
       <c r="G44">
         <v>0.4217013248878961</v>
@@ -1820,7 +1820,7 @@
         <v>-0.1268230767511501</v>
       </c>
       <c r="I44">
-        <v>1.129094456372921</v>
+        <v>1.162927453616514</v>
       </c>
     </row>
     <row r="45">
@@ -1841,10 +1841,10 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0.5027723836321715</v>
+        <v>0.2749150350482624</v>
       </c>
       <c r="F45">
-        <v>1.569564403911113</v>
+        <v>1.621412486903809</v>
       </c>
       <c r="G45">
         <v>-0.7703781740154796</v>
@@ -1853,7 +1853,7 @@
         <v>0.1901146834763395</v>
       </c>
       <c r="I45">
-        <v>1.083035874171312</v>
+        <v>0.8551785255874025</v>
       </c>
     </row>
     <row r="46">
@@ -1874,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.487526907927867</v>
+        <v>0.3390178850367488</v>
       </c>
       <c r="F46">
-        <v>1.044954852369915</v>
+        <v>1.010829853119227</v>
       </c>
       <c r="G46">
         <v>0.1696321872222053</v>
@@ -1886,7 +1886,7 @@
         <v>-0.696185701270406</v>
       </c>
       <c r="I46">
-        <v>1.014080421976068</v>
+        <v>0.8655713990849495</v>
       </c>
     </row>
     <row r="47">
@@ -1907,10 +1907,10 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>-1.228254788739885</v>
+        <v>-1.334903493104364</v>
       </c>
       <c r="F47">
-        <v>0.296504301832453</v>
+        <v>0.1842087821834784</v>
       </c>
       <c r="G47">
         <v>0.1684697069789879</v>
@@ -1919,7 +1919,7 @@
         <v>-1.191274748505505</v>
       </c>
       <c r="I47">
-        <v>-0.2054497472133684</v>
+        <v>-0.3120984515778472</v>
       </c>
     </row>
     <row r="48">
@@ -1940,10 +1940,10 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>-1.033495696102753</v>
+        <v>-1.20934288059607</v>
       </c>
       <c r="F48">
-        <v>-0.3178627983206519</v>
+        <v>-0.482578363403854</v>
       </c>
       <c r="G48">
         <v>0.01859064452557019</v>
@@ -1952,7 +1952,7 @@
         <v>-0.5812383154098705</v>
       </c>
       <c r="I48">
-        <v>-0.4708480252184526</v>
+        <v>-0.6466952097117696</v>
       </c>
     </row>
     <row r="49">
@@ -1973,10 +1973,10 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>-1.844211867209407</v>
+        <v>-2.053992548263863</v>
       </c>
       <c r="F49">
-        <v>-0.9046088610310465</v>
+        <v>-1.064805259231885</v>
       </c>
       <c r="G49">
         <v>0.844913545254637</v>
@@ -1985,7 +1985,7 @@
         <v>-2.013634932113948</v>
       </c>
       <c r="I49">
-        <v>-0.6754904803500962</v>
+        <v>-0.885271161404552</v>
       </c>
     </row>
     <row r="50">
@@ -2006,10 +2006,10 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>-0.7923170903823507</v>
+        <v>-0.9230959876344373</v>
       </c>
       <c r="F50">
-        <v>-1.224569860608601</v>
+        <v>-1.380333727399682</v>
       </c>
       <c r="G50">
         <v>0.2562045734879467</v>
@@ -2018,7 +2018,7 @@
         <v>-0.3122102720358756</v>
       </c>
       <c r="I50">
-        <v>-0.7363113918344216</v>
+        <v>-0.8670902890865084</v>
       </c>
     </row>
     <row r="51">
@@ -2039,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>-1.169355210949045</v>
+        <v>-1.284328665377682</v>
       </c>
       <c r="F51">
-        <v>-1.209844966160891</v>
+        <v>-1.367690020468011</v>
       </c>
       <c r="G51">
         <v>0.1450182149398946</v>
@@ -2051,7 +2051,7 @@
         <v>-0.4947906108575231</v>
       </c>
       <c r="I51">
-        <v>-0.8195828150314167</v>
+        <v>-0.9345562694600537</v>
       </c>
     </row>
     <row r="52">
@@ -2072,10 +2072,10 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>-0.9639806311531158</v>
+        <v>-1.135870449807741</v>
       </c>
       <c r="F52">
-        <v>-1.192466199923482</v>
+        <v>-1.349321912770929</v>
       </c>
       <c r="G52">
         <v>-0.4323678523936096</v>
@@ -2084,7 +2084,7 @@
         <v>0.02432447663671006</v>
       </c>
       <c r="I52">
-        <v>-0.5559372553962162</v>
+        <v>-0.7278270740508411</v>
       </c>
     </row>
     <row r="53">
@@ -2105,10 +2105,10 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>-0.5440837190432699</v>
+        <v>-0.7354084543804134</v>
       </c>
       <c r="F53">
-        <v>-0.8674341628819477</v>
+        <v>-1.019675889300067</v>
       </c>
       <c r="G53">
         <v>0.3803818637273209</v>
@@ -2117,7 +2117,7 @@
         <v>-0.5017904711965351</v>
       </c>
       <c r="I53">
-        <v>-0.4226751115740557</v>
+        <v>-0.6139998469111991</v>
       </c>
     </row>
     <row r="54">
@@ -2138,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>-1.270416700125953</v>
+        <v>-1.395908815178557</v>
       </c>
       <c r="F54">
-        <v>-0.9869590653178483</v>
+        <v>-1.137879096186097</v>
       </c>
       <c r="G54">
         <v>-0.6673024455224547</v>
@@ -2150,7 +2150,7 @@
         <v>-0.09428784992988173</v>
       </c>
       <c r="I54">
-        <v>-0.5088264046736169</v>
+        <v>-0.6343185197262209</v>
       </c>
     </row>
     <row r="55">
@@ -2171,10 +2171,10 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>-1.501064206101111</v>
+        <v>-1.603357517632246</v>
       </c>
       <c r="F55">
-        <v>-1.069886314105865</v>
+        <v>-1.217636309249738</v>
       </c>
       <c r="G55">
         <v>-0.4174472957211435</v>
@@ -2183,7 +2183,7 @@
         <v>-0.2709188102602541</v>
       </c>
       <c r="I55">
-        <v>-0.812698100119714</v>
+        <v>-0.914991411650849</v>
       </c>
     </row>
     <row r="56">
@@ -2204,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>-0.9942887050768487</v>
+        <v>-1.116499933729532</v>
       </c>
       <c r="F56">
-        <v>-1.077463332586798</v>
+        <v>-1.212793680230186</v>
       </c>
       <c r="G56">
         <v>-0.5559174319186626</v>
@@ -2216,7 +2216,7 @@
         <v>0.4227614915339761</v>
       </c>
       <c r="I56">
-        <v>-0.8611327646921623</v>
+        <v>-0.9833439933448452</v>
       </c>
     </row>
     <row r="57">
@@ -2237,10 +2237,10 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>-0.8480800902533412</v>
+        <v>-0.9726691887561941</v>
       </c>
       <c r="F57">
-        <v>-1.153462425389316</v>
+        <v>-1.272108863824131</v>
       </c>
       <c r="G57">
         <v>-0.2997224000918609</v>
@@ -2249,7 +2249,7 @@
         <v>-0.1045155710692038</v>
       </c>
       <c r="I57">
-        <v>-0.4438421190922766</v>
+        <v>-0.5684312175951295</v>
       </c>
     </row>
     <row r="58">
@@ -2270,10 +2270,10 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>-1.094797389213942</v>
+        <v>-1.187728961935022</v>
       </c>
       <c r="F58">
-        <v>-1.109557597661313</v>
+        <v>-1.220063900513247</v>
       </c>
       <c r="G58">
         <v>-0.2240111183472178</v>
@@ -2282,7 +2282,7 @@
         <v>-0.3661740621074557</v>
       </c>
       <c r="I58">
-        <v>-0.5046122087592682</v>
+        <v>-0.5975437814803488</v>
       </c>
     </row>
     <row r="59">
@@ -2303,10 +2303,10 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>-0.9873392427980625</v>
+        <v>-1.193308975962579</v>
       </c>
       <c r="F59">
-        <v>-0.9811263568355508</v>
+        <v>-1.117551765095831</v>
       </c>
       <c r="G59">
         <v>-0.4061811825802247</v>
@@ -2315,7 +2315,7 @@
         <v>0.0958164009158845</v>
       </c>
       <c r="I59">
-        <v>-0.6769744611337223</v>
+        <v>-0.8829441942982384</v>
       </c>
     </row>
     <row r="60">
@@ -2336,10 +2336,10 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>-0.4337172435729012</v>
+        <v>-0.6534648789357949</v>
       </c>
       <c r="F60">
-        <v>-0.840983491459564</v>
+        <v>-1.001793001397397</v>
       </c>
       <c r="G60">
         <v>-0.7509726066732845</v>
@@ -2348,7 +2348,7 @@
         <v>0.8413517740071288</v>
       </c>
       <c r="I60">
-        <v>-0.5240964109067455</v>
+        <v>-0.7438440462696392</v>
       </c>
     </row>
     <row r="61">
@@ -2369,10 +2369,10 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>0.06818610730826508</v>
+        <v>0.01928216522450138</v>
       </c>
       <c r="F61">
-        <v>-0.6119169420691624</v>
+        <v>-0.7538051629022228</v>
       </c>
       <c r="G61">
         <v>-0.0812099604090557</v>
@@ -2381,7 +2381,7 @@
         <v>0.5670893333084116</v>
       </c>
       <c r="I61">
-        <v>-0.4176932655910908</v>
+        <v>-0.4665972076748545</v>
       </c>
     </row>
     <row r="62">
@@ -2402,10 +2402,10 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>-0.3138305920119502</v>
+        <v>-0.3344821017130632</v>
       </c>
       <c r="F62">
-        <v>-0.4166752427686645</v>
+        <v>-0.540493447846733</v>
       </c>
       <c r="G62">
         <v>-0.1957491219772411</v>
@@ -2414,7 +2414,7 @@
         <v>0.1610420819330972</v>
       </c>
       <c r="I62">
-        <v>-0.2791235519678062</v>
+        <v>-0.2997750616689193</v>
       </c>
     </row>
     <row r="63">
@@ -2435,10 +2435,10 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0.3586091394787078</v>
+        <v>0.3140609946513788</v>
       </c>
       <c r="F63">
-        <v>-0.08018814719947187</v>
+        <v>-0.1636509551932436</v>
       </c>
       <c r="G63">
         <v>-0.4074660776168579</v>
@@ -2447,7 +2447,7 @@
         <v>0.7737859440606548</v>
       </c>
       <c r="I63">
-        <v>-0.007710726965089121</v>
+        <v>-0.05225887179241816</v>
       </c>
     </row>
     <row r="64">
@@ -2468,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0.5752689314829336</v>
+        <v>0.529034318439913</v>
       </c>
       <c r="F64">
-        <v>0.1720583965644868</v>
+        <v>0.1319738441506833</v>
       </c>
       <c r="G64">
         <v>0.06277798709953475</v>
@@ -2480,7 +2480,7 @@
         <v>0.5420811257918118</v>
       </c>
       <c r="I64">
-        <v>-0.02959018140841301</v>
+        <v>-0.07582479445143357</v>
       </c>
     </row>
     <row r="65">
@@ -2501,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0.3107163185030594</v>
+        <v>0.2954484137361119</v>
       </c>
       <c r="F65">
-        <v>0.2326909493631854</v>
+        <v>0.2010154062785859</v>
       </c>
       <c r="G65">
         <v>-0.1327573957763631</v>
@@ -2513,7 +2513,7 @@
         <v>0.4514429786931769</v>
       </c>
       <c r="I65">
-        <v>-0.007969264413754397</v>
+        <v>-0.02323716918070192</v>
       </c>
     </row>
     <row r="66">
@@ -2534,10 +2534,10 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0.1647850815238155</v>
+        <v>0.1592797295325848</v>
       </c>
       <c r="F66">
-        <v>0.3523448677471269</v>
+        <v>0.3244558640899979</v>
       </c>
       <c r="G66">
         <v>-0.1801940834457704</v>
@@ -2546,7 +2546,7 @@
         <v>0.4351408046902969</v>
       </c>
       <c r="I66">
-        <v>-0.09016163972071101</v>
+        <v>-0.09566699171194178</v>
       </c>
     </row>
     <row r="67">
@@ -2567,10 +2567,10 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>0.5807596919664175</v>
+        <v>0.5804714712727042</v>
       </c>
       <c r="F67">
-        <v>0.4078825058690543</v>
+        <v>0.3910584832453293</v>
       </c>
       <c r="G67">
         <v>0.1446360764488608</v>
@@ -2579,7 +2579,7 @@
         <v>0.5046954554173962</v>
       </c>
       <c r="I67">
-        <v>-0.0685718398998395</v>
+        <v>-0.06886006059355292</v>
       </c>
     </row>
     <row r="68">
@@ -2600,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>-0.2197921669657434</v>
+        <v>-0.2211301141010897</v>
       </c>
       <c r="F68">
-        <v>0.209117231256885</v>
+        <v>0.2035173751100786</v>
       </c>
       <c r="G68">
         <v>-0.3900965921543058</v>
@@ -2612,7 +2612,7 @@
         <v>0.2771373206810341</v>
       </c>
       <c r="I68">
-        <v>-0.1068328954924717</v>
+        <v>-0.108170842627818</v>
       </c>
     </row>
     <row r="69">
@@ -2633,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>0.1587899660362987</v>
+        <v>0.152867248038262</v>
       </c>
       <c r="F69">
-        <v>0.1711356431401949</v>
+        <v>0.1678720836856161</v>
       </c>
       <c r="G69">
         <v>-0.08733488089964167</v>
@@ -2645,7 +2645,7 @@
         <v>0.4167077288083179</v>
       </c>
       <c r="I69">
-        <v>-0.1705828818723776</v>
+        <v>-0.1765055998704143</v>
       </c>
     </row>
     <row r="70">
@@ -2666,10 +2666,10 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>0.04697945168012474</v>
+        <v>0.03499534418986899</v>
       </c>
       <c r="F70">
-        <v>0.1416842356792722</v>
+        <v>0.1368009873499372</v>
       </c>
       <c r="G70">
         <v>-0.1278436839455424</v>
@@ -2678,7 +2678,7 @@
         <v>0.3139223053663386</v>
       </c>
       <c r="I70">
-        <v>-0.1390991697406714</v>
+        <v>-0.1510832772309272</v>
       </c>
     </row>
     <row r="71">
@@ -2699,10 +2699,10 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0.03063398948661511</v>
+        <v>0.01581406170779704</v>
       </c>
       <c r="F71">
-        <v>0.004152810059321554</v>
+        <v>-0.004363365041289591</v>
       </c>
       <c r="G71">
         <v>0.2677292251719238</v>
@@ -2711,7 +2711,7 @@
         <v>-0.263229069689987</v>
       </c>
       <c r="I71">
-        <v>0.02613383400467834</v>
+        <v>0.01131390622586027</v>
       </c>
     </row>
     <row r="72">
@@ -2732,10 +2732,10 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0.3184515106945939</v>
+        <v>0.3067301817554395</v>
       </c>
       <c r="F72">
-        <v>0.1387137294744059</v>
+        <v>0.1276017089228427</v>
       </c>
       <c r="G72">
         <v>0.52312767676769</v>
@@ -2744,7 +2744,7 @@
         <v>-0.2543557166457277</v>
       </c>
       <c r="I72">
-        <v>0.04967955057263165</v>
+        <v>0.03795822163347724</v>
       </c>
     </row>
     <row r="73">
@@ -2765,10 +2765,10 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>0.0270230738796577</v>
+        <v>0.02112093191430813</v>
       </c>
       <c r="F73">
-        <v>0.1057720064352457</v>
+        <v>0.09466512989185424</v>
       </c>
       <c r="G73">
         <v>-0.2462085424130513</v>
@@ -2777,7 +2777,7 @@
         <v>0.2811655584663052</v>
       </c>
       <c r="I73">
-        <v>-0.007933942173596206</v>
+        <v>-0.01383608413894578</v>
       </c>
     </row>
     <row r="74">
@@ -2798,10 +2798,10 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0.3032190477306695</v>
+        <v>0.296149184554314</v>
       </c>
       <c r="F74">
-        <v>0.1698319054478819</v>
+        <v>0.1599535899829655</v>
       </c>
       <c r="G74">
         <v>0.2626719596059693</v>
@@ -2810,7 +2810,7 @@
         <v>0.2304793770639839</v>
       </c>
       <c r="I74">
-        <v>-0.1899322889392836</v>
+        <v>-0.1970021521156391</v>
       </c>
     </row>
     <row r="75">
@@ -2831,10 +2831,10 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0.2949461609358204</v>
+        <v>0.2802196829059673</v>
       </c>
       <c r="F75">
-        <v>0.2359099483101832</v>
+        <v>0.2260549952825081</v>
       </c>
       <c r="G75">
         <v>0.08774199681802211</v>
@@ -2843,7 +2843,7 @@
         <v>0.1651340442225374</v>
       </c>
       <c r="I75">
-        <v>0.04207011989526092</v>
+        <v>0.02734364186540785</v>
       </c>
     </row>
     <row r="76">
@@ -2864,10 +2864,10 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0.715023170604688</v>
+        <v>0.6948359934315428</v>
       </c>
       <c r="F76">
-        <v>0.3350528632877067</v>
+        <v>0.3230814482015338</v>
       </c>
       <c r="G76">
         <v>0.4297577362167462</v>
@@ -2876,7 +2876,7 @@
         <v>0.07225776655800209</v>
       </c>
       <c r="I76">
-        <v>0.2130076678299398</v>
+        <v>0.1928204906567945</v>
       </c>
     </row>
     <row r="77">
@@ -2897,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0.458753367945863</v>
+        <v>0.4423585520343201</v>
       </c>
       <c r="F77">
-        <v>0.4429854368042581</v>
+        <v>0.4283908532315368</v>
       </c>
       <c r="G77">
         <v>0.2109924963445054</v>
@@ -2909,7 +2909,7 @@
         <v>0.226214317730833</v>
       </c>
       <c r="I77">
-        <v>0.0215465538705246</v>
+        <v>0.005151737958981705</v>
       </c>
     </row>
     <row r="78">
@@ -2930,10 +2930,10 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>-0.1144843406281816</v>
+        <v>-0.122414152362562</v>
       </c>
       <c r="F78">
-        <v>0.3385595897145453</v>
+        <v>0.3237500190023178</v>
       </c>
       <c r="G78">
         <v>0.237122930151244</v>
@@ -2942,7 +2942,7 @@
         <v>-0.3937263151375531</v>
       </c>
       <c r="I78">
-        <v>0.04211904435812747</v>
+        <v>0.03418923262374703</v>
       </c>
     </row>
     <row r="79">
@@ -2963,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0.5105071087186668</v>
+        <v>0.5133099992348448</v>
       </c>
       <c r="F79">
-        <v>0.3924498266602569</v>
+        <v>0.3820225980845371</v>
       </c>
       <c r="G79">
         <v>-0.1472996337848166</v>
@@ -2975,7 +2975,7 @@
         <v>0.5780486871037616</v>
       </c>
       <c r="I79">
-        <v>0.07975805539972179</v>
+        <v>0.08256094591589977</v>
       </c>
     </row>
     <row r="80">
@@ -2996,10 +2996,10 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>0.9040497598393208</v>
+        <v>0.9033371672225152</v>
       </c>
       <c r="F80">
-        <v>0.439706473968915</v>
+        <v>0.4341478915322803</v>
       </c>
       <c r="G80">
         <v>0.3571800727378065</v>
@@ -3008,7 +3008,7 @@
         <v>0.502883685661647</v>
       </c>
       <c r="I80">
-        <v>0.04398600143986734</v>
+        <v>0.04327340882306176</v>
       </c>
     </row>
     <row r="81">
@@ -3029,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>0.7130188020751458</v>
+        <v>0.7040338335519547</v>
       </c>
       <c r="F81">
-        <v>0.5032728325012358</v>
+        <v>0.4995667119116889</v>
       </c>
       <c r="G81">
         <v>0.3494500224676224</v>
@@ -3041,7 +3041,7 @@
         <v>0.02425579270840394</v>
       </c>
       <c r="I81">
-        <v>0.3393129868991195</v>
+        <v>0.3303280183759284</v>
       </c>
     </row>
     <row r="82">
@@ -3062,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <v>0.7870438773809589</v>
+        <v>0.7864500408666604</v>
       </c>
       <c r="F82">
-        <v>0.728654887003521</v>
+        <v>0.7267827602189946</v>
       </c>
       <c r="G82">
         <v>0.212703570123558</v>
@@ -3074,7 +3074,7 @@
         <v>0.2037445872558542</v>
       </c>
       <c r="I82">
-        <v>0.3705957200015467</v>
+        <v>0.3700018834872481</v>
       </c>
     </row>
     <row r="83">
@@ -3095,10 +3095,10 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>0.3547449270644294</v>
+        <v>0.4723158052048929</v>
       </c>
       <c r="F83">
-        <v>0.6897143415899616</v>
+        <v>0.7165342117115067</v>
       </c>
       <c r="G83">
         <v>-0.067915184401038</v>
@@ -3107,7 +3107,7 @@
         <v>0.2893119225244437</v>
       </c>
       <c r="I83">
-        <v>0.1333481889410237</v>
+        <v>0.2509190670814871</v>
       </c>
     </row>
     <row r="84">
@@ -3128,19 +3128,19 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>14.38875125218292</v>
+        <v>26.6240649623621</v>
       </c>
       <c r="F84">
-        <v>4.060889714675862</v>
+        <v>7.146716160496402</v>
       </c>
       <c r="G84">
-        <v>-13.31659129694795</v>
+        <v>7.417972338488096</v>
       </c>
       <c r="H84">
-        <v>13.75712049673779</v>
+        <v>-6.977443138698249</v>
       </c>
       <c r="I84">
-        <v>13.94822205239307</v>
+        <v>26.18353576257225</v>
       </c>
     </row>
     <row r="85">
@@ -3161,19 +3161,19 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>5.687626540253732</v>
+        <v>6.672164248622796</v>
       </c>
       <c r="F85">
-        <v>5.304541649220509</v>
+        <v>8.638748764264113</v>
       </c>
       <c r="G85">
-        <v>13.49528513621632</v>
+        <v>-0.6059559168268347</v>
       </c>
       <c r="H85">
-        <v>-14.39457650423646</v>
+        <v>-0.2933354511933026</v>
       </c>
       <c r="I85">
-        <v>6.586917908273869</v>
+        <v>7.571455616642933</v>
       </c>
     </row>
     <row r="86">
@@ -3191,19 +3191,19 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <v>11.23486937091637</v>
+        <v>-9.888477807369904</v>
       </c>
       <c r="F86">
-        <v>7.916498022604362</v>
+        <v>5.970016802204972</v>
       </c>
       <c r="G86">
-        <v>-2.596242575697091</v>
+        <v>-10.95445077968873</v>
       </c>
       <c r="H86">
-        <v>2.665547952690785</v>
+        <v>11.02375615668243</v>
       </c>
       <c r="I86">
-        <v>11.16556399392268</v>
+        <v>-9.957783184363599</v>
       </c>
     </row>
     <row r="87">
@@ -3221,10 +3221,10 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>10.76235316171048</v>
+        <v>-6.78929843281013</v>
       </c>
       <c r="F87">
-        <v>10.51840008126587</v>
+        <v>4.154613242701216</v>
       </c>
       <c r="G87">
         <v>0.0211449975886567</v>
@@ -3233,7 +3233,7 @@
         <v>-0.0489758373568531</v>
       </c>
       <c r="I87">
-        <v>10.79018400147867</v>
+        <v>-6.761467593041934</v>
       </c>
     </row>
     <row r="88">
@@ -3251,10 +3251,10 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>2.389343138774026</v>
+        <v>-7.225268809517935</v>
       </c>
       <c r="F88">
-        <v>7.518548052913649</v>
+        <v>-4.307720200268792</v>
       </c>
       <c r="G88">
         <v>0.4455684743108141</v>
@@ -3263,7 +3263,7 @@
         <v>-0.6095921842875095</v>
       </c>
       <c r="I88">
-        <v>2.553366848750722</v>
+        <v>-7.06124509954124</v>
       </c>
     </row>
     <row r="89">
@@ -3281,10 +3281,10 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>5.494067414004169</v>
+        <v>-7.506627702180698</v>
       </c>
       <c r="F89">
-        <v>7.470158271351259</v>
+        <v>-7.852418187969666</v>
       </c>
       <c r="G89">
         <v>-0.5275958895402297</v>
@@ -3293,7 +3293,7 @@
         <v>0.5211163550401237</v>
       </c>
       <c r="I89">
-        <v>5.500546948504275</v>
+        <v>-7.500148167680592</v>
       </c>
     </row>
     <row r="90">
@@ -3311,10 +3311,10 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>0.1065563638982546</v>
+        <v>-4.929671961345584</v>
       </c>
       <c r="F90">
-        <v>4.68808001959673</v>
+        <v>-6.612716726463587</v>
       </c>
       <c r="G90">
         <v>0.6207551504777457</v>
@@ -3323,7 +3323,7 @@
         <v>-0.4561486085349057</v>
       </c>
       <c r="I90">
-        <v>-0.05805017804458534</v>
+        <v>-5.094278503288424</v>
       </c>
     </row>
     <row r="91">
@@ -3341,10 +3341,10 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>0.1374038155831119</v>
+        <v>-3.139676406377838</v>
       </c>
       <c r="F91">
-        <v>2.031842683064889</v>
+        <v>-5.700311219855513</v>
       </c>
       <c r="G91">
         <v>0.6462216737799427</v>
@@ -3353,7 +3353,7 @@
         <v>-0.4081564310641782</v>
       </c>
       <c r="I91">
-        <v>-0.1006614271326526</v>
+        <v>-3.377741649093603</v>
       </c>
     </row>
     <row r="92">
@@ -3371,10 +3371,10 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <v>0.2425736764547175</v>
+        <v>-4.786424135282775</v>
       </c>
       <c r="F92">
-        <v>1.495150317485062</v>
+        <v>-5.090600051296724</v>
       </c>
       <c r="G92">
         <v>0.4402212415595376</v>
@@ -3383,7 +3383,7 @@
         <v>-0.1992292447670816</v>
       </c>
       <c r="I92">
-        <v>0.001581679662261526</v>
+        <v>-5.027416132075231</v>
       </c>
     </row>
     <row r="93">
@@ -3401,10 +3401,10 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <v>1.802257175914217</v>
+        <v>-2.148736098348152</v>
       </c>
       <c r="F93">
-        <v>0.5721977579625737</v>
+        <v>-3.751127150338587</v>
       </c>
       <c r="G93">
         <v>0.4647309823073583</v>
@@ -3413,7 +3413,7 @@
         <v>-0.2593821185563237</v>
       </c>
       <c r="I93">
-        <v>1.596908312163182</v>
+        <v>-2.354084962099187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>